<commit_message>
Accuracy and repeatability calculations
</commit_message>
<xml_diff>
--- a/docs/testplan/SAT_TEMPLATE_v0_1_after_coll.xlsx
+++ b/docs/testplan/SAT_TEMPLATE_v0_1_after_coll.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="176">
   <si>
     <t>General Inspection</t>
   </si>
@@ -550,6 +550,12 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Max value=</t>
+  </si>
+  <si>
+    <t>Average=</t>
   </si>
 </sst>
 </file>
@@ -558,8 +564,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.0000E+00"/>
-    <numFmt numFmtId="185" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1249,7 +1255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1414,17 +1420,17 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1453,11 +1459,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1492,13 +1496,21 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="185" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="185" fontId="9" fillId="0" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3658,7 +3670,7 @@
   <dimension ref="A2:AA124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3725,7 +3737,7 @@
       <c r="J6" s="88" t="s">
         <v>109</v>
       </c>
-      <c r="K6" s="89" t="s">
+      <c r="L6" s="89" t="s">
         <v>24</v>
       </c>
       <c r="N6" s="54" t="s">
@@ -3767,7 +3779,13 @@
       <c r="J7" s="82">
         <v>8.1062348299999997E-5</v>
       </c>
-      <c r="K7" s="80"/>
+      <c r="K7" s="154" t="s">
+        <v>174</v>
+      </c>
+      <c r="L7" s="155">
+        <f>MAX(F7:F11)</f>
+        <v>5.6566004136456627E-2</v>
+      </c>
       <c r="N7" s="68"/>
       <c r="O7" s="69"/>
       <c r="P7" s="69"/>
@@ -3803,7 +3821,13 @@
       <c r="J8" s="83">
         <v>30.726190200000001</v>
       </c>
-      <c r="K8" s="81"/>
+      <c r="K8" s="154" t="s">
+        <v>175</v>
+      </c>
+      <c r="L8" s="156">
+        <f>AVERAGE(F7:F11)</f>
+        <v>4.9680461078188951E-2</v>
+      </c>
       <c r="N8" s="58">
         <v>5</v>
       </c>
@@ -3878,7 +3902,7 @@
         <f>$I$7*D22</f>
         <v>40.022640337869682</v>
       </c>
-      <c r="E11" s="115">
+      <c r="E11" s="152">
         <f>ABS((ABS($I$8)*F27)+$J$8)</f>
         <v>39.969970467047702</v>
       </c>
@@ -3943,7 +3967,7 @@
       <c r="H16" t="s">
         <v>164</v>
       </c>
-      <c r="I16" s="84">
+      <c r="I16" s="112">
         <v>691207</v>
       </c>
       <c r="J16">
@@ -3981,7 +4005,7 @@
       <c r="E18" s="112">
         <v>691215</v>
       </c>
-      <c r="F18" s="117"/>
+      <c r="F18" s="116"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C19" s="51">
@@ -3993,7 +4017,7 @@
       <c r="E19" s="112">
         <v>466367</v>
       </c>
-      <c r="F19" s="117"/>
+      <c r="F19" s="116"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C20" s="51">
@@ -4005,7 +4029,7 @@
       <c r="E20" s="114">
         <v>241664</v>
       </c>
-      <c r="F20" s="118"/>
+      <c r="F20" s="117"/>
     </row>
     <row r="21" spans="1:27" s="108" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="51">
@@ -4017,7 +4041,7 @@
       <c r="E21" s="112">
         <v>17199</v>
       </c>
-      <c r="F21" s="117"/>
+      <c r="F21" s="116"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C22" s="51">
@@ -4026,10 +4050,10 @@
       <c r="D22" s="110">
         <v>493726.6336</v>
       </c>
-      <c r="E22" s="115">
+      <c r="E22" s="151">
         <v>2147276036</v>
       </c>
-      <c r="F22" s="116"/>
+      <c r="F22" s="115"/>
     </row>
     <row r="23" spans="1:27" s="79" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23"/>
@@ -4155,7 +4179,7 @@
       <c r="E27">
         <v>2147483647</v>
       </c>
-      <c r="F27" s="119">
+      <c r="F27" s="153">
         <f>E27-E22</f>
         <v>207611</v>
       </c>
@@ -4630,97 +4654,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" style="125"/>
-    <col min="2" max="2" width="11.796875" style="125" customWidth="1"/>
-    <col min="3" max="4" width="21.5" style="125" customWidth="1"/>
-    <col min="5" max="5" width="18.69921875" style="125" customWidth="1"/>
-    <col min="6" max="6" width="16.796875" style="125" customWidth="1"/>
-    <col min="7" max="7" width="13.69921875" style="125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.19921875" style="125" customWidth="1"/>
-    <col min="9" max="16384" width="11.19921875" style="125"/>
+    <col min="1" max="1" width="11.19921875" style="123"/>
+    <col min="2" max="2" width="11.796875" style="123" customWidth="1"/>
+    <col min="3" max="4" width="21.5" style="123" customWidth="1"/>
+    <col min="5" max="5" width="18.69921875" style="123" customWidth="1"/>
+    <col min="6" max="6" width="16.796875" style="123" customWidth="1"/>
+    <col min="7" max="7" width="13.69921875" style="123" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.19921875" style="123" customWidth="1"/>
+    <col min="9" max="16384" width="11.19921875" style="123"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120">
+      <c r="C2" s="118"/>
+      <c r="D2" s="118">
         <v>6</v>
       </c>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B3" s="120" t="s">
+      <c r="B3" s="118" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120" t="s">
+      <c r="C3" s="118"/>
+      <c r="D3" s="118" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="120"/>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B4" s="120"/>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120" t="s">
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
+      <c r="D4" s="118" t="s">
         <v>171</v>
       </c>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
-      <c r="G4" s="120"/>
-      <c r="H4" s="120"/>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="118"/>
+      <c r="I4" s="118"/>
+      <c r="J4" s="118"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B5" s="120"/>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="118"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="118"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B6" s="120" t="s">
+      <c r="B6" s="118" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="120"/>
-      <c r="D6" s="120">
+      <c r="C6" s="118"/>
+      <c r="D6" s="118">
         <v>-5</v>
       </c>
-      <c r="E6" s="120">
+      <c r="E6" s="118">
         <v>0</v>
       </c>
-      <c r="F6" s="120">
+      <c r="F6" s="118">
         <v>10</v>
       </c>
-      <c r="G6" s="120">
+      <c r="G6" s="118">
         <v>20</v>
       </c>
-      <c r="H6" s="120">
+      <c r="H6" s="118">
         <v>30</v>
       </c>
-      <c r="I6" s="120">
+      <c r="I6" s="118">
         <v>40</v>
       </c>
     </row>
@@ -4728,37 +4752,37 @@
       <c r="M8"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B9" s="120"/>
-      <c r="C9" s="126"/>
-      <c r="D9" s="126"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="124"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
       <c r="M9"/>
-      <c r="N9" s="139" t="s">
+      <c r="N9" s="137" t="s">
         <v>73</v>
       </c>
-      <c r="O9" s="127" t="s">
+      <c r="O9" s="125" t="s">
         <v>74</v>
       </c>
-      <c r="P9" s="127"/>
-      <c r="Q9" s="127"/>
-      <c r="R9" s="127"/>
-      <c r="S9" s="127"/>
-      <c r="T9" s="127"/>
-      <c r="U9" s="128"/>
+      <c r="P9" s="125"/>
+      <c r="Q9" s="125"/>
+      <c r="R9" s="125"/>
+      <c r="S9" s="125"/>
+      <c r="T9" s="125"/>
+      <c r="U9" s="126"/>
     </row>
     <row r="10" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="120" t="s">
+      <c r="B10" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="126" t="s">
+      <c r="C10" s="124" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="126"/>
-      <c r="E10" s="120" t="s">
+      <c r="D10" s="124"/>
+      <c r="E10" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="120"/>
+      <c r="F10" s="118"/>
       <c r="H10" t="s">
         <v>158</v>
       </c>
@@ -4766,29 +4790,29 @@
       <c r="J10"/>
       <c r="K10"/>
       <c r="M10"/>
-      <c r="N10" s="131"/>
-      <c r="O10" s="132"/>
-      <c r="P10" s="132"/>
-      <c r="Q10" s="132"/>
-      <c r="R10" s="132"/>
-      <c r="S10" s="132"/>
-      <c r="T10" s="132"/>
-      <c r="U10" s="133"/>
+      <c r="N10" s="129"/>
+      <c r="O10" s="130"/>
+      <c r="P10" s="130"/>
+      <c r="Q10" s="130"/>
+      <c r="R10" s="130"/>
+      <c r="S10" s="130"/>
+      <c r="T10" s="130"/>
+      <c r="U10" s="131"/>
     </row>
     <row r="11" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="141" t="s">
+      <c r="B11" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="142" t="s">
+      <c r="C11" s="140" t="s">
         <v>162</v>
       </c>
-      <c r="D11" s="142" t="s">
+      <c r="D11" s="140" t="s">
         <v>170</v>
       </c>
-      <c r="E11" s="142" t="s">
+      <c r="E11" s="140" t="s">
         <v>169</v>
       </c>
-      <c r="F11" s="143" t="s">
+      <c r="F11" s="141" t="s">
         <v>37</v>
       </c>
       <c r="H11" s="86"/>
@@ -4802,29 +4826,29 @@
         <v>24</v>
       </c>
       <c r="M11"/>
-      <c r="N11" s="135"/>
-      <c r="O11" s="132"/>
-      <c r="P11" s="132"/>
-      <c r="Q11" s="132"/>
-      <c r="R11" s="132"/>
-      <c r="S11" s="132"/>
-      <c r="T11" s="133"/>
+      <c r="N11" s="133"/>
+      <c r="O11" s="130"/>
+      <c r="P11" s="130"/>
+      <c r="Q11" s="130"/>
+      <c r="R11" s="130"/>
+      <c r="S11" s="130"/>
+      <c r="T11" s="131"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B12" s="144">
+      <c r="B12" s="142">
         <v>1</v>
       </c>
-      <c r="C12" s="140">
+      <c r="C12" s="138">
         <v>-4.2187500000000003E-2</v>
       </c>
-      <c r="D12" s="150">
+      <c r="D12" s="148">
         <f>$I$12*C12</f>
         <v>-3.4198178189062502E-6</v>
       </c>
-      <c r="E12" s="122">
+      <c r="E12" s="120">
         <v>691215</v>
       </c>
-      <c r="F12" s="123">
+      <c r="F12" s="121">
         <f>ABS((ABS($I$13)*E12)-$J$13)</f>
         <v>4.9826375650496857E-2</v>
       </c>
@@ -4839,29 +4863,29 @@
       </c>
       <c r="K12" s="80"/>
       <c r="M12"/>
-      <c r="N12" s="135"/>
-      <c r="O12" s="132"/>
-      <c r="P12" s="132"/>
-      <c r="Q12" s="132"/>
-      <c r="R12" s="132"/>
-      <c r="S12" s="132"/>
-      <c r="T12" s="133"/>
+      <c r="N12" s="133"/>
+      <c r="O12" s="130"/>
+      <c r="P12" s="130"/>
+      <c r="Q12" s="130"/>
+      <c r="R12" s="130"/>
+      <c r="S12" s="130"/>
+      <c r="T12" s="131"/>
     </row>
     <row r="13" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="144">
+      <c r="B13" s="142">
         <v>2</v>
       </c>
-      <c r="C13" s="140">
+      <c r="C13" s="138">
         <v>-4.2187500000000003E-2</v>
       </c>
-      <c r="D13" s="150">
+      <c r="D13" s="148">
         <f t="shared" ref="D13:D15" si="0">$I$12*C13</f>
         <v>-3.4198178189062502E-6</v>
       </c>
-      <c r="E13" s="140">
+      <c r="E13" s="138">
         <v>691212</v>
       </c>
-      <c r="F13" s="123">
+      <c r="F13" s="121">
         <f t="shared" ref="F13:F15" si="1">ABS((ABS($I$13)*E13)-$J$13)</f>
         <v>4.9692802088397769E-2</v>
       </c>
@@ -4876,1567 +4900,1567 @@
       </c>
       <c r="K13" s="81"/>
       <c r="M13"/>
-      <c r="N13" s="135"/>
-      <c r="O13" s="132"/>
-      <c r="P13" s="132"/>
-      <c r="Q13" s="132"/>
-      <c r="R13" s="132"/>
-      <c r="S13" s="132"/>
-      <c r="T13" s="133"/>
+      <c r="N13" s="133"/>
+      <c r="O13" s="130"/>
+      <c r="P13" s="130"/>
+      <c r="Q13" s="130"/>
+      <c r="R13" s="130"/>
+      <c r="S13" s="130"/>
+      <c r="T13" s="131"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B14" s="144">
+      <c r="B14" s="142">
         <v>3</v>
       </c>
-      <c r="C14" s="140">
+      <c r="C14" s="138">
         <v>-4.9218749999999999E-2</v>
       </c>
-      <c r="D14" s="150">
+      <c r="D14" s="148">
         <f t="shared" si="0"/>
         <v>-3.9897874553906247E-6</v>
       </c>
-      <c r="E14" s="140">
+      <c r="E14" s="138">
         <v>691212</v>
       </c>
-      <c r="F14" s="123">
+      <c r="F14" s="121">
         <f t="shared" si="1"/>
         <v>4.9692802088397769E-2</v>
       </c>
       <c r="M14"/>
-      <c r="N14" s="135"/>
-      <c r="O14" s="132"/>
-      <c r="P14" s="132"/>
-      <c r="Q14" s="132"/>
-      <c r="R14" s="132"/>
-      <c r="S14" s="132"/>
-      <c r="T14" s="133"/>
+      <c r="N14" s="133"/>
+      <c r="O14" s="130"/>
+      <c r="P14" s="130"/>
+      <c r="Q14" s="130"/>
+      <c r="R14" s="130"/>
+      <c r="S14" s="130"/>
+      <c r="T14" s="131"/>
     </row>
     <row r="15" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="145">
+      <c r="B15" s="143">
         <v>4</v>
       </c>
-      <c r="C15" s="146">
+      <c r="C15" s="144">
         <v>-4.9218749999999999E-2</v>
       </c>
-      <c r="D15" s="150">
+      <c r="D15" s="148">
         <f t="shared" si="0"/>
         <v>-3.9897874553906247E-6</v>
       </c>
-      <c r="E15" s="146">
+      <c r="E15" s="144">
         <v>691212</v>
       </c>
-      <c r="F15" s="123">
+      <c r="F15" s="121">
         <f t="shared" si="1"/>
         <v>4.9692802088397769E-2</v>
       </c>
       <c r="M15"/>
-      <c r="N15" s="135"/>
-      <c r="O15" s="132"/>
-      <c r="P15" s="132"/>
-      <c r="Q15" s="132"/>
-      <c r="R15" s="132"/>
-      <c r="S15" s="132"/>
-      <c r="T15" s="133"/>
+      <c r="N15" s="133"/>
+      <c r="O15" s="130"/>
+      <c r="P15" s="130"/>
+      <c r="Q15" s="130"/>
+      <c r="R15" s="130"/>
+      <c r="S15" s="130"/>
+      <c r="T15" s="131"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B16" s="141" t="s">
+      <c r="B16" s="139" t="s">
         <v>114</v>
       </c>
-      <c r="D16" s="151">
+      <c r="D16" s="149">
         <f>MAX(D12:D15)-MIN(D12:D15)</f>
         <v>5.6996963648437454E-7</v>
       </c>
-      <c r="F16" s="121">
+      <c r="F16" s="119">
         <f>MAX(F12:F15)-MIN(F12:F15)</f>
         <v>1.3357356209908744E-4</v>
       </c>
       <c r="M16"/>
-      <c r="N16" s="135"/>
-      <c r="O16" s="132"/>
-      <c r="P16" s="132"/>
-      <c r="Q16" s="132"/>
-      <c r="R16" s="132"/>
-      <c r="S16" s="132"/>
-      <c r="T16" s="133"/>
+      <c r="N16" s="133"/>
+      <c r="O16" s="130"/>
+      <c r="P16" s="130"/>
+      <c r="Q16" s="130"/>
+      <c r="R16" s="130"/>
+      <c r="S16" s="130"/>
+      <c r="T16" s="131"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B17" s="144" t="s">
+      <c r="B17" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="D17" s="122">
+      <c r="D17" s="120">
         <f>STDEV(C12:C15)</f>
         <v>4.059494080239554E-3</v>
       </c>
-      <c r="F17" s="122">
+      <c r="F17" s="120">
         <f>STDEV(F12:F15)</f>
         <v>6.678678104954372E-5</v>
       </c>
-      <c r="I17" s="129" t="s">
+      <c r="I17" s="127" t="s">
         <v>117</v>
       </c>
-      <c r="J17" s="130"/>
+      <c r="J17" s="128"/>
       <c r="M17"/>
-      <c r="N17" s="135"/>
-      <c r="O17" s="132"/>
-      <c r="P17" s="132"/>
-      <c r="Q17" s="132"/>
-      <c r="R17" s="132"/>
-      <c r="S17" s="132"/>
-      <c r="T17" s="133"/>
+      <c r="N17" s="133"/>
+      <c r="O17" s="130"/>
+      <c r="P17" s="130"/>
+      <c r="Q17" s="130"/>
+      <c r="R17" s="130"/>
+      <c r="S17" s="130"/>
+      <c r="T17" s="131"/>
     </row>
     <row r="18" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="145" t="s">
+      <c r="B18" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="147">
+      <c r="C18" s="145">
         <f>MAX(D16:F16)</f>
         <v>1.3357356209908744E-4</v>
       </c>
-      <c r="D18" s="149"/>
-      <c r="E18" s="148"/>
-      <c r="F18" s="124"/>
-      <c r="H18" s="125" t="s">
+      <c r="D18" s="147"/>
+      <c r="E18" s="146"/>
+      <c r="F18" s="122"/>
+      <c r="H18" s="123" t="s">
         <v>172</v>
       </c>
-      <c r="I18" s="134">
+      <c r="I18" s="132">
         <f>MAX(C18,C28,C38,C50,C62,C74,C86,C98,C110,C122)</f>
         <v>9.3501493469716479E-4</v>
       </c>
       <c r="M18"/>
-      <c r="N18" s="135"/>
-      <c r="O18" s="132"/>
-      <c r="P18" s="132"/>
-      <c r="Q18" s="132"/>
-      <c r="R18" s="132"/>
-      <c r="S18" s="132"/>
-      <c r="T18" s="132"/>
-      <c r="U18" s="133"/>
+      <c r="N18" s="133"/>
+      <c r="O18" s="130"/>
+      <c r="P18" s="130"/>
+      <c r="Q18" s="130"/>
+      <c r="R18" s="130"/>
+      <c r="S18" s="130"/>
+      <c r="T18" s="130"/>
+      <c r="U18" s="131"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.3">
       <c r="H19" t="s">
         <v>173</v>
       </c>
-      <c r="I19" s="134">
+      <c r="I19" s="132">
         <f>AVERAGE(C18,C28,C38,C50,C62,C74,C86,C98,C110,C122)</f>
         <v>6.0108102944944619E-4</v>
       </c>
       <c r="M19"/>
-      <c r="N19" s="135"/>
-      <c r="O19" s="132"/>
-      <c r="P19" s="132"/>
-      <c r="Q19" s="132"/>
-      <c r="R19" s="132"/>
-      <c r="S19" s="132"/>
-      <c r="T19" s="132"/>
-      <c r="U19" s="133"/>
+      <c r="N19" s="133"/>
+      <c r="O19" s="130"/>
+      <c r="P19" s="130"/>
+      <c r="Q19" s="130"/>
+      <c r="R19" s="130"/>
+      <c r="S19" s="130"/>
+      <c r="T19" s="130"/>
+      <c r="U19" s="131"/>
     </row>
     <row r="20" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="120" t="s">
+      <c r="B20" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="126" t="s">
+      <c r="C20" s="124" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="126"/>
-      <c r="E20" s="120" t="s">
+      <c r="D20" s="124"/>
+      <c r="E20" s="118" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="120"/>
+      <c r="F20" s="118"/>
       <c r="M20"/>
-      <c r="N20" s="135"/>
-      <c r="O20" s="132"/>
-      <c r="P20" s="132"/>
-      <c r="Q20" s="132"/>
-      <c r="R20" s="132"/>
-      <c r="S20" s="132"/>
-      <c r="T20" s="132"/>
-      <c r="U20" s="133"/>
+      <c r="N20" s="133"/>
+      <c r="O20" s="130"/>
+      <c r="P20" s="130"/>
+      <c r="Q20" s="130"/>
+      <c r="R20" s="130"/>
+      <c r="S20" s="130"/>
+      <c r="T20" s="130"/>
+      <c r="U20" s="131"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B21" s="141" t="s">
+      <c r="B21" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="142" t="s">
+      <c r="C21" s="140" t="s">
         <v>162</v>
       </c>
-      <c r="D21" s="142" t="s">
+      <c r="D21" s="140" t="s">
         <v>170</v>
       </c>
-      <c r="E21" s="142" t="s">
+      <c r="E21" s="140" t="s">
         <v>169</v>
       </c>
-      <c r="F21" s="143" t="s">
+      <c r="F21" s="141" t="s">
         <v>37</v>
       </c>
       <c r="M21"/>
-      <c r="N21" s="135"/>
-      <c r="O21" s="132"/>
-      <c r="P21" s="132"/>
-      <c r="Q21" s="132"/>
-      <c r="R21" s="132"/>
-      <c r="S21" s="132"/>
-      <c r="T21" s="133"/>
+      <c r="N21" s="133"/>
+      <c r="O21" s="130"/>
+      <c r="P21" s="130"/>
+      <c r="Q21" s="130"/>
+      <c r="R21" s="130"/>
+      <c r="S21" s="130"/>
+      <c r="T21" s="131"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B22" s="144">
+      <c r="B22" s="142">
         <v>1</v>
       </c>
-      <c r="C22" s="140">
+      <c r="C22" s="138">
         <v>4.9218749999999999E-2</v>
       </c>
-      <c r="D22" s="150">
+      <c r="D22" s="148">
         <f>$I$12*C22</f>
         <v>3.9897874553906247E-6</v>
       </c>
-      <c r="E22" s="122">
+      <c r="E22" s="120">
         <v>690520</v>
       </c>
-      <c r="F22" s="123">
+      <c r="F22" s="121">
         <f>ABS((ABS($I$13)*E22)-$J$13)</f>
         <v>1.8881833763998657E-2</v>
       </c>
       <c r="M22"/>
-      <c r="N22" s="135"/>
-      <c r="O22" s="132"/>
-      <c r="P22" s="132"/>
-      <c r="Q22" s="132"/>
-      <c r="R22" s="132"/>
-      <c r="S22" s="132"/>
-      <c r="T22" s="133"/>
+      <c r="N22" s="133"/>
+      <c r="O22" s="130"/>
+      <c r="P22" s="130"/>
+      <c r="Q22" s="130"/>
+      <c r="R22" s="130"/>
+      <c r="S22" s="130"/>
+      <c r="T22" s="131"/>
     </row>
     <row r="23" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="144">
+      <c r="B23" s="142">
         <v>2</v>
       </c>
-      <c r="C23" s="140">
+      <c r="C23" s="138">
         <v>4.2187500000000003E-2</v>
       </c>
-      <c r="D23" s="150">
+      <c r="D23" s="148">
         <f t="shared" ref="D23:D25" si="2">$I$12*C23</f>
         <v>3.4198178189062502E-6</v>
       </c>
-      <c r="E23" s="140">
+      <c r="E23" s="138">
         <v>690512</v>
       </c>
-      <c r="F23" s="123">
+      <c r="F23" s="121">
         <f t="shared" ref="F23:F25" si="3">ABS((ABS($I$13)*E23)-$J$13)</f>
         <v>1.8525637598397537E-2</v>
       </c>
       <c r="M23"/>
-      <c r="N23" s="136"/>
-      <c r="O23" s="137"/>
-      <c r="P23" s="137"/>
-      <c r="Q23" s="137"/>
-      <c r="R23" s="137"/>
-      <c r="S23" s="137"/>
-      <c r="T23" s="138"/>
+      <c r="N23" s="134"/>
+      <c r="O23" s="135"/>
+      <c r="P23" s="135"/>
+      <c r="Q23" s="135"/>
+      <c r="R23" s="135"/>
+      <c r="S23" s="135"/>
+      <c r="T23" s="136"/>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B24" s="144">
+      <c r="B24" s="142">
         <v>3</v>
       </c>
-      <c r="C24" s="140">
+      <c r="C24" s="138">
         <v>4.2187500000000003E-2</v>
       </c>
-      <c r="D24" s="150">
+      <c r="D24" s="148">
         <f t="shared" si="2"/>
         <v>3.4198178189062502E-6</v>
       </c>
-      <c r="E24" s="140">
+      <c r="E24" s="138">
         <v>690511</v>
       </c>
-      <c r="F24" s="123">
+      <c r="F24" s="121">
         <f t="shared" si="3"/>
         <v>1.8481113077697842E-2</v>
       </c>
     </row>
     <row r="25" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="145">
+      <c r="B25" s="143">
         <v>4</v>
       </c>
-      <c r="C25" s="146">
+      <c r="C25" s="144">
         <v>4.2187500000000003E-2</v>
       </c>
-      <c r="D25" s="150">
+      <c r="D25" s="148">
         <f t="shared" si="2"/>
         <v>3.4198178189062502E-6</v>
       </c>
-      <c r="E25" s="146">
+      <c r="E25" s="144">
         <v>690507</v>
       </c>
-      <c r="F25" s="123">
+      <c r="F25" s="121">
         <f t="shared" si="3"/>
         <v>1.8303014994899058E-2</v>
       </c>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B26" s="141" t="s">
+      <c r="B26" s="139" t="s">
         <v>114</v>
       </c>
-      <c r="D26" s="151">
+      <c r="D26" s="149">
         <f>MAX(D22:D25)-MIN(D22:D25)</f>
         <v>5.6996963648437454E-7</v>
       </c>
-      <c r="F26" s="121">
+      <c r="F26" s="119">
         <f>MAX(F22:F25)-MIN(F22:F25)</f>
         <v>5.7881876909959828E-4</v>
       </c>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B27" s="144" t="s">
+      <c r="B27" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="D27" s="122">
+      <c r="D27" s="120">
         <f>STDEV(C22:C25)</f>
         <v>3.5156249999999979E-3</v>
       </c>
-      <c r="F27" s="122">
+      <c r="F27" s="120">
         <f>STDEV(F22:F25)</f>
         <v>2.4251222098224437E-4</v>
       </c>
     </row>
     <row r="28" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="145" t="s">
+      <c r="B28" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="C28" s="147">
+      <c r="C28" s="145">
         <f>MAX(D26:F26)</f>
         <v>5.7881876909959828E-4</v>
       </c>
-      <c r="D28" s="149"/>
-      <c r="E28" s="148"/>
-      <c r="F28" s="124"/>
+      <c r="D28" s="147"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="122"/>
     </row>
     <row r="30" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="120" t="s">
+      <c r="B30" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="126" t="s">
+      <c r="C30" s="124" t="s">
         <v>81</v>
       </c>
-      <c r="D30" s="126"/>
-      <c r="E30" s="120" t="s">
+      <c r="D30" s="124"/>
+      <c r="E30" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="F30" s="120"/>
+      <c r="F30" s="118"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B31" s="141" t="s">
+      <c r="B31" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="142" t="s">
+      <c r="C31" s="140" t="s">
         <v>162</v>
       </c>
-      <c r="D31" s="142" t="s">
+      <c r="D31" s="140" t="s">
         <v>170</v>
       </c>
-      <c r="E31" s="142" t="s">
+      <c r="E31" s="140" t="s">
         <v>169</v>
       </c>
-      <c r="F31" s="143" t="s">
+      <c r="F31" s="141" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B32" s="144">
+      <c r="B32" s="142">
         <v>1</v>
       </c>
-      <c r="C32" s="140">
+      <c r="C32" s="138">
         <v>123431.625</v>
       </c>
-      <c r="D32" s="150">
+      <c r="D32" s="148">
         <f>$I$12*C32</f>
         <v>10.005657376984987</v>
       </c>
-      <c r="E32" s="122">
+      <c r="E32" s="120">
         <v>466367</v>
       </c>
-      <c r="F32" s="123">
+      <c r="F32" s="121">
         <f>ABS((ABS($I$13)*E32)-$J$13)</f>
         <v>9.9614230547031006</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B33" s="144">
+      <c r="B33" s="142">
         <v>2</v>
       </c>
-      <c r="C33" s="140">
+      <c r="C33" s="138">
         <v>123431.625</v>
       </c>
-      <c r="D33" s="150">
+      <c r="D33" s="148">
         <f t="shared" ref="D33:D35" si="4">$I$12*C33</f>
         <v>10.005657376984987</v>
       </c>
-      <c r="E33" s="140">
+      <c r="E33" s="138">
         <v>466352</v>
       </c>
-      <c r="F33" s="123">
+      <c r="F33" s="121">
         <f t="shared" ref="F33:F35" si="5">ABS((ABS($I$13)*E33)-$J$13)</f>
         <v>9.9620909225136032</v>
       </c>
-      <c r="L33" s="120"/>
+      <c r="L33" s="118"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B34" s="144">
+      <c r="B34" s="142">
         <v>3</v>
       </c>
-      <c r="C34" s="140">
+      <c r="C34" s="138">
         <v>123431.625</v>
       </c>
-      <c r="D34" s="150">
+      <c r="D34" s="148">
         <f t="shared" si="4"/>
         <v>10.005657376984987</v>
       </c>
-      <c r="E34" s="140">
+      <c r="E34" s="138">
         <v>466359</v>
       </c>
-      <c r="F34" s="123">
+      <c r="F34" s="121">
         <f t="shared" si="5"/>
         <v>9.9617792508687018</v>
       </c>
-      <c r="L34" s="126"/>
+      <c r="L34" s="124"/>
     </row>
     <row r="35" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="145">
+      <c r="B35" s="143">
         <v>4</v>
       </c>
-      <c r="C35" s="146">
+      <c r="C35" s="144">
         <v>123431.625</v>
       </c>
-      <c r="D35" s="150">
+      <c r="D35" s="148">
         <f t="shared" si="4"/>
         <v>10.005657376984987</v>
       </c>
-      <c r="E35" s="146">
+      <c r="E35" s="144">
         <v>466363</v>
       </c>
-      <c r="F35" s="123">
+      <c r="F35" s="121">
         <f t="shared" si="5"/>
         <v>9.961601152785903</v>
       </c>
-      <c r="L35" s="120"/>
+      <c r="L35" s="118"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B36" s="141" t="s">
+      <c r="B36" s="139" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="151">
+      <c r="D36" s="149">
         <f>MAX(D32:D35)-MIN(D32:D35)</f>
         <v>0</v>
       </c>
-      <c r="F36" s="121">
+      <c r="F36" s="119">
         <f>MAX(F32:F35)-MIN(F32:F35)</f>
         <v>6.6786781050254262E-4</v>
       </c>
-      <c r="L36" s="120"/>
+      <c r="L36" s="118"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B37" s="144" t="s">
+      <c r="B37" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="122">
+      <c r="D37" s="120">
         <f>STDEV(C32:C35)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="122">
+      <c r="F37" s="120">
         <f>STDEV(F32:F35)</f>
         <v>2.848061585382772E-4</v>
       </c>
-      <c r="L37" s="120"/>
+      <c r="L37" s="118"/>
     </row>
     <row r="38" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="145" t="s">
+      <c r="B38" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="C38" s="147">
+      <c r="C38" s="145">
         <f>MAX(D36:F36)</f>
         <v>6.6786781050254262E-4</v>
       </c>
-      <c r="D38" s="149"/>
-      <c r="E38" s="148"/>
-      <c r="F38" s="124"/>
-      <c r="L38" s="120"/>
+      <c r="D38" s="147"/>
+      <c r="E38" s="146"/>
+      <c r="F38" s="122"/>
+      <c r="L38" s="118"/>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="L39" s="120"/>
+      <c r="L39" s="118"/>
     </row>
     <row r="42" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="120" t="s">
+      <c r="B42" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="126" t="s">
+      <c r="C42" s="124" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="126"/>
-      <c r="E42" s="120" t="s">
+      <c r="D42" s="124"/>
+      <c r="E42" s="118" t="s">
         <v>79</v>
       </c>
-      <c r="F42" s="120"/>
+      <c r="F42" s="118"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B43" s="141" t="s">
+      <c r="B43" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="142" t="s">
+      <c r="C43" s="140" t="s">
         <v>162</v>
       </c>
-      <c r="D43" s="142" t="s">
+      <c r="D43" s="140" t="s">
         <v>170</v>
       </c>
-      <c r="E43" s="142" t="s">
+      <c r="E43" s="140" t="s">
         <v>169</v>
       </c>
-      <c r="F43" s="143" t="s">
+      <c r="F43" s="141" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B44" s="144">
+      <c r="B44" s="142">
         <v>1</v>
       </c>
-      <c r="C44" s="140">
+      <c r="C44" s="138">
         <v>123431.70940000001</v>
       </c>
-      <c r="D44" s="150">
+      <c r="D44" s="148">
         <f>$I$12*C44</f>
         <v>10.005664218647185</v>
       </c>
-      <c r="E44" s="122">
+      <c r="E44" s="120">
         <v>465771</v>
       </c>
-      <c r="F44" s="123">
+      <c r="F44" s="121">
         <f>ABS((ABS($I$13)*E44)-$J$13)</f>
         <v>9.9879596690403005</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B45" s="144">
+      <c r="B45" s="142">
         <v>2</v>
       </c>
-      <c r="C45" s="140">
+      <c r="C45" s="138">
         <v>123431.70940000001</v>
       </c>
-      <c r="D45" s="150">
+      <c r="D45" s="148">
         <f t="shared" ref="D45:D47" si="6">$I$12*C45</f>
         <v>10.005664218647185</v>
       </c>
-      <c r="E45" s="140">
+      <c r="E45" s="138">
         <v>465767</v>
       </c>
-      <c r="F45" s="123">
+      <c r="F45" s="121">
         <f t="shared" ref="F45:F47" si="7">ABS((ABS($I$13)*E45)-$J$13)</f>
         <v>9.9881377671231029</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B46" s="144">
+      <c r="B46" s="142">
         <v>3</v>
       </c>
-      <c r="C46" s="140">
+      <c r="C46" s="138">
         <v>123431.70940000001</v>
       </c>
-      <c r="D46" s="150">
+      <c r="D46" s="148">
         <f t="shared" si="6"/>
         <v>10.005664218647185</v>
       </c>
-      <c r="E46" s="140">
+      <c r="E46" s="138">
         <v>465763</v>
       </c>
-      <c r="F46" s="123">
+      <c r="F46" s="121">
         <f t="shared" si="7"/>
         <v>9.9883158652059016</v>
       </c>
     </row>
     <row r="47" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="145">
+      <c r="B47" s="143">
         <v>4</v>
       </c>
-      <c r="C47" s="146">
+      <c r="C47" s="144">
         <v>123431.7164</v>
       </c>
-      <c r="D47" s="150">
+      <c r="D47" s="148">
         <f t="shared" si="6"/>
         <v>10.005664786083623</v>
       </c>
-      <c r="E47" s="146">
+      <c r="E47" s="144">
         <v>465759</v>
       </c>
-      <c r="F47" s="123">
+      <c r="F47" s="121">
         <f t="shared" si="7"/>
         <v>9.9884939632887004</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B48" s="141" t="s">
+      <c r="B48" s="139" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="151">
+      <c r="D48" s="149">
         <f>MAX(D44:D47)-MIN(D44:D47)</f>
         <v>5.6743643739309846E-7</v>
       </c>
-      <c r="F48" s="121">
+      <c r="F48" s="119">
         <f>MAX(F44:F47)-MIN(F44:F47)</f>
         <v>5.3429424839990247E-4</v>
       </c>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B49" s="144" t="s">
+      <c r="B49" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="D49" s="122">
+      <c r="D49" s="120">
         <f>STDEV(C44:C47)</f>
         <v>3.4999999988940544E-3</v>
       </c>
-      <c r="F49" s="122">
+      <c r="F49" s="120">
         <f>STDEV(F44:F47)</f>
         <v>2.29923636225095E-4</v>
       </c>
     </row>
     <row r="50" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="145" t="s">
+      <c r="B50" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="C50" s="147">
+      <c r="C50" s="145">
         <f>MAX(D48:F48)</f>
         <v>5.3429424839990247E-4</v>
       </c>
-      <c r="D50" s="149"/>
-      <c r="E50" s="148"/>
-      <c r="F50" s="124"/>
+      <c r="D50" s="147"/>
+      <c r="E50" s="146"/>
+      <c r="F50" s="122"/>
     </row>
     <row r="54" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="120" t="s">
+      <c r="B54" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="C54" s="120" t="s">
+      <c r="C54" s="118" t="s">
         <v>82</v>
       </c>
-      <c r="D54" s="120"/>
-      <c r="E54" s="120" t="s">
+      <c r="D54" s="118"/>
+      <c r="E54" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="F54" s="120"/>
+      <c r="F54" s="118"/>
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B55" s="141" t="s">
+      <c r="B55" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="C55" s="142" t="s">
+      <c r="C55" s="140" t="s">
         <v>162</v>
       </c>
-      <c r="D55" s="142" t="s">
+      <c r="D55" s="140" t="s">
         <v>170</v>
       </c>
-      <c r="E55" s="142" t="s">
+      <c r="E55" s="140" t="s">
         <v>169</v>
       </c>
-      <c r="F55" s="143" t="s">
+      <c r="F55" s="141" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="56" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B56" s="144">
+      <c r="B56" s="142">
         <v>1</v>
       </c>
-      <c r="C56" s="140">
+      <c r="C56" s="138">
         <v>246863.29920000001</v>
       </c>
-      <c r="D56" s="150">
+      <c r="D56" s="148">
         <f>$I$12*C56</f>
         <v>20.01131874223751</v>
       </c>
-      <c r="E56" s="122">
+      <c r="E56" s="120">
         <v>241664</v>
       </c>
-      <c r="F56" s="123">
+      <c r="F56" s="121">
         <f>ABS((ABS($I$13)*E56)-$J$13)</f>
         <v>19.966216429555203</v>
       </c>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B57" s="144">
+      <c r="B57" s="142">
         <v>2</v>
       </c>
-      <c r="C57" s="152">
+      <c r="C57" s="150">
         <v>246863.2922</v>
       </c>
-      <c r="D57" s="150">
+      <c r="D57" s="148">
         <f t="shared" ref="D57:D59" si="8">$I$12*C57</f>
         <v>20.011318174801072</v>
       </c>
-      <c r="E57" s="140">
+      <c r="E57" s="138">
         <v>241656</v>
       </c>
-      <c r="F57" s="123">
+      <c r="F57" s="121">
         <f t="shared" ref="F57:F59" si="9">ABS((ABS($I$13)*E57)-$J$13)</f>
         <v>19.966572625720801</v>
       </c>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B58" s="144">
+      <c r="B58" s="142">
         <v>3</v>
       </c>
-      <c r="C58" s="140">
+      <c r="C58" s="138">
         <v>246863.29920000001</v>
       </c>
-      <c r="D58" s="150">
+      <c r="D58" s="148">
         <f t="shared" si="8"/>
         <v>20.01131874223751</v>
       </c>
-      <c r="E58" s="140">
+      <c r="E58" s="138">
         <v>241663</v>
       </c>
-      <c r="F58" s="123">
+      <c r="F58" s="121">
         <f t="shared" si="9"/>
         <v>19.966260954075899</v>
       </c>
-      <c r="K58" s="120"/>
-      <c r="S58" s="120"/>
+      <c r="K58" s="118"/>
+      <c r="S58" s="118"/>
     </row>
     <row r="59" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="145">
+      <c r="B59" s="143">
         <v>4</v>
       </c>
-      <c r="C59" s="146">
+      <c r="C59" s="144">
         <v>246863.29920000001</v>
       </c>
-      <c r="D59" s="150">
+      <c r="D59" s="148">
         <f t="shared" si="8"/>
         <v>20.01131874223751</v>
       </c>
-      <c r="E59" s="146">
+      <c r="E59" s="144">
         <v>241668</v>
       </c>
-      <c r="F59" s="123">
+      <c r="F59" s="121">
         <f t="shared" si="9"/>
         <v>19.966038331472401</v>
       </c>
-      <c r="K59" s="126"/>
-      <c r="S59" s="120"/>
+      <c r="K59" s="124"/>
+      <c r="S59" s="118"/>
     </row>
     <row r="60" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B60" s="141" t="s">
+      <c r="B60" s="139" t="s">
         <v>114</v>
       </c>
-      <c r="D60" s="151">
+      <c r="D60" s="149">
         <f>MAX(D56:D59)-MIN(D56:D59)</f>
         <v>5.6743643739309846E-7</v>
       </c>
-      <c r="F60" s="121">
+      <c r="F60" s="119">
         <f>MAX(F56:F59)-MIN(F56:F59)</f>
         <v>5.3429424839990247E-4</v>
       </c>
-      <c r="K60" s="120"/>
-      <c r="S60" s="120"/>
+      <c r="K60" s="118"/>
+      <c r="S60" s="118"/>
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B61" s="144" t="s">
+      <c r="B61" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="D61" s="122">
+      <c r="D61" s="120">
         <f>STDEV(C56:C59)</f>
         <v>3.5000000061700116E-3</v>
       </c>
-      <c r="F61" s="122">
+      <c r="F61" s="120">
         <f>STDEV(F56:F59)</f>
         <v>2.2225125611281983E-4</v>
       </c>
-      <c r="K61" s="120"/>
-      <c r="S61" s="120"/>
+      <c r="K61" s="118"/>
+      <c r="S61" s="118"/>
     </row>
     <row r="62" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="145" t="s">
+      <c r="B62" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="C62" s="147">
+      <c r="C62" s="145">
         <f>MAX(D60:F60)</f>
         <v>5.3429424839990247E-4</v>
       </c>
-      <c r="D62" s="149"/>
-      <c r="E62" s="148"/>
-      <c r="F62" s="124"/>
-      <c r="K62" s="120"/>
-      <c r="S62" s="120"/>
+      <c r="D62" s="147"/>
+      <c r="E62" s="146"/>
+      <c r="F62" s="122"/>
+      <c r="K62" s="118"/>
+      <c r="S62" s="118"/>
     </row>
     <row r="63" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="K63" s="120"/>
-      <c r="S63" s="120"/>
+      <c r="K63" s="118"/>
+      <c r="S63" s="118"/>
     </row>
     <row r="64" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="K64" s="120"/>
-      <c r="S64" s="120"/>
+      <c r="K64" s="118"/>
+      <c r="S64" s="118"/>
     </row>
     <row r="66" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="120" t="s">
+      <c r="B66" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="C66" s="120" t="s">
+      <c r="C66" s="118" t="s">
         <v>82</v>
       </c>
-      <c r="D66" s="120"/>
-      <c r="E66" s="120" t="s">
+      <c r="D66" s="118"/>
+      <c r="E66" s="118" t="s">
         <v>79</v>
       </c>
-      <c r="F66" s="120"/>
+      <c r="F66" s="118"/>
     </row>
     <row r="67" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B67" s="141" t="s">
+      <c r="B67" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="C67" s="142" t="s">
+      <c r="C67" s="140" t="s">
         <v>162</v>
       </c>
-      <c r="D67" s="142" t="s">
+      <c r="D67" s="140" t="s">
         <v>170</v>
       </c>
-      <c r="E67" s="142" t="s">
+      <c r="E67" s="140" t="s">
         <v>169</v>
       </c>
-      <c r="F67" s="143" t="s">
+      <c r="F67" s="141" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B68" s="144">
+      <c r="B68" s="142">
         <v>1</v>
       </c>
-      <c r="C68" s="140">
+      <c r="C68" s="138">
         <v>246863.3836</v>
       </c>
-      <c r="D68" s="150">
+      <c r="D68" s="148">
         <f>$I$12*C68</f>
         <v>20.011325583899708</v>
       </c>
-      <c r="E68" s="122">
+      <c r="E68" s="120">
         <v>241192</v>
       </c>
-      <c r="F68" s="123">
+      <c r="F68" s="121">
         <f>ABS((ABS($I$13)*E68)-$J$13)</f>
         <v>19.987232003325602</v>
       </c>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B69" s="144">
+      <c r="B69" s="142">
         <v>2</v>
       </c>
-      <c r="C69" s="140">
+      <c r="C69" s="138">
         <v>246863.3836</v>
       </c>
-      <c r="D69" s="150">
+      <c r="D69" s="148">
         <f t="shared" ref="D69:D71" si="10">$I$12*C69</f>
         <v>20.011325583899708</v>
       </c>
-      <c r="E69" s="140">
+      <c r="E69" s="138">
         <v>241188</v>
       </c>
-      <c r="F69" s="123">
+      <c r="F69" s="121">
         <f t="shared" ref="F69:F71" si="11">ABS((ABS($I$13)*E69)-$J$13)</f>
         <v>19.9874101014084</v>
       </c>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B70" s="144">
+      <c r="B70" s="142">
         <v>3</v>
       </c>
-      <c r="C70" s="140">
+      <c r="C70" s="138">
         <v>246863.3836</v>
       </c>
-      <c r="D70" s="150">
+      <c r="D70" s="148">
         <f t="shared" si="10"/>
         <v>20.011325583899708</v>
       </c>
-      <c r="E70" s="140">
+      <c r="E70" s="138">
         <v>241184</v>
       </c>
-      <c r="F70" s="123">
+      <c r="F70" s="121">
         <f t="shared" si="11"/>
         <v>19.987588199491199</v>
       </c>
     </row>
     <row r="71" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="145">
+      <c r="B71" s="143">
         <v>4</v>
       </c>
-      <c r="C71" s="146">
+      <c r="C71" s="144">
         <v>246863.3836</v>
       </c>
-      <c r="D71" s="150">
+      <c r="D71" s="148">
         <f t="shared" si="10"/>
         <v>20.011325583899708</v>
       </c>
-      <c r="E71" s="146">
+      <c r="E71" s="144">
         <v>241180</v>
       </c>
-      <c r="F71" s="123">
+      <c r="F71" s="121">
         <f t="shared" si="11"/>
         <v>19.987766297574002</v>
       </c>
     </row>
     <row r="72" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B72" s="141" t="s">
+      <c r="B72" s="139" t="s">
         <v>114</v>
       </c>
-      <c r="D72" s="151">
+      <c r="D72" s="149">
         <f>MAX(D68:D71)-MIN(D68:D71)</f>
         <v>0</v>
       </c>
-      <c r="F72" s="121">
+      <c r="F72" s="119">
         <f>MAX(F68:F71)-MIN(F68:F71)</f>
         <v>5.3429424839990247E-4</v>
       </c>
     </row>
     <row r="73" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B73" s="144" t="s">
+      <c r="B73" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="D73" s="122">
+      <c r="D73" s="120">
         <f>STDEV(C68:C71)</f>
         <v>0</v>
       </c>
-      <c r="F73" s="122">
+      <c r="F73" s="120">
         <f>STDEV(F68:F71)</f>
         <v>2.29923636225095E-4</v>
       </c>
     </row>
     <row r="74" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="145" t="s">
+      <c r="B74" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="C74" s="147">
+      <c r="C74" s="145">
         <f>MAX(D72:F72)</f>
         <v>5.3429424839990247E-4</v>
       </c>
-      <c r="D74" s="149"/>
-      <c r="E74" s="148"/>
-      <c r="F74" s="124"/>
+      <c r="D74" s="147"/>
+      <c r="E74" s="146"/>
+      <c r="F74" s="122"/>
     </row>
     <row r="77" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="S77" s="120"/>
+      <c r="S77" s="118"/>
     </row>
     <row r="78" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="120" t="s">
+      <c r="B78" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="C78" s="120" t="s">
+      <c r="C78" s="118" t="s">
         <v>83</v>
       </c>
-      <c r="D78" s="120"/>
-      <c r="E78" s="120" t="s">
+      <c r="D78" s="118"/>
+      <c r="E78" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="F78" s="120"/>
-      <c r="S78" s="120"/>
+      <c r="F78" s="118"/>
+      <c r="S78" s="118"/>
     </row>
     <row r="79" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B79" s="141" t="s">
+      <c r="B79" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="C79" s="142" t="s">
+      <c r="C79" s="140" t="s">
         <v>162</v>
       </c>
-      <c r="D79" s="142" t="s">
+      <c r="D79" s="140" t="s">
         <v>170</v>
       </c>
-      <c r="E79" s="142" t="s">
+      <c r="E79" s="140" t="s">
         <v>169</v>
       </c>
-      <c r="F79" s="143" t="s">
+      <c r="F79" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="S79" s="120"/>
+      <c r="S79" s="118"/>
     </row>
     <row r="80" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B80" s="144">
+      <c r="B80" s="142">
         <v>1</v>
       </c>
-      <c r="C80" s="140">
+      <c r="C80" s="138">
         <v>370294.95939999999</v>
       </c>
-      <c r="D80" s="150">
+      <c r="D80" s="148">
         <f>$I$12*C80</f>
         <v>30.016978972617157</v>
       </c>
-      <c r="E80" s="122">
+      <c r="E80" s="120">
         <v>17199</v>
       </c>
-      <c r="F80" s="123">
+      <c r="F80" s="121">
         <f>ABS((ABS($I$13)*E80)-$J$13)</f>
         <v>29.9604129684807</v>
       </c>
-      <c r="S80" s="120"/>
+      <c r="S80" s="118"/>
     </row>
     <row r="81" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B81" s="144">
+      <c r="B81" s="142">
         <v>2</v>
       </c>
-      <c r="C81" s="140">
+      <c r="C81" s="138">
         <v>370294.95939999999</v>
       </c>
-      <c r="D81" s="150">
+      <c r="D81" s="148">
         <f t="shared" ref="D81:D83" si="12">$I$12*C81</f>
         <v>30.016978972617157</v>
       </c>
-      <c r="E81" s="140">
+      <c r="E81" s="138">
         <v>17180</v>
       </c>
-      <c r="F81" s="123">
+      <c r="F81" s="121">
         <f t="shared" ref="F81:F83" si="13">ABS((ABS($I$13)*E81)-$J$13)</f>
         <v>29.961258934374001</v>
       </c>
-      <c r="S81" s="120"/>
+      <c r="S81" s="118"/>
     </row>
     <row r="82" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B82" s="144">
+      <c r="B82" s="142">
         <v>3</v>
       </c>
-      <c r="C82" s="140">
+      <c r="C82" s="138">
         <v>370294.96639999998</v>
       </c>
-      <c r="D82" s="150">
+      <c r="D82" s="148">
         <f t="shared" si="12"/>
         <v>30.016979540053594</v>
       </c>
-      <c r="E82" s="140">
+      <c r="E82" s="138">
         <v>17184</v>
       </c>
-      <c r="F82" s="123">
+      <c r="F82" s="121">
         <f t="shared" si="13"/>
         <v>29.961080836291202</v>
       </c>
-      <c r="S82" s="120"/>
+      <c r="S82" s="118"/>
     </row>
     <row r="83" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="145">
+      <c r="B83" s="143">
         <v>4</v>
       </c>
-      <c r="C83" s="146">
+      <c r="C83" s="144">
         <v>370294.96639999998</v>
       </c>
-      <c r="D83" s="150">
+      <c r="D83" s="148">
         <f t="shared" si="12"/>
         <v>30.016979540053594</v>
       </c>
-      <c r="E83" s="146">
+      <c r="E83" s="144">
         <v>17184</v>
       </c>
-      <c r="F83" s="123">
+      <c r="F83" s="121">
         <f t="shared" si="13"/>
         <v>29.961080836291202</v>
       </c>
-      <c r="S83" s="120"/>
+      <c r="S83" s="118"/>
     </row>
     <row r="84" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B84" s="141" t="s">
+      <c r="B84" s="139" t="s">
         <v>114</v>
       </c>
-      <c r="D84" s="151">
+      <c r="D84" s="149">
         <f>MAX(D80:D83)-MIN(D80:D83)</f>
         <v>5.6743643739309846E-7</v>
       </c>
-      <c r="F84" s="121">
+      <c r="F84" s="119">
         <f>MAX(F80:F83)-MIN(F80:F83)</f>
         <v>8.4596589330132588E-4</v>
       </c>
-      <c r="S84" s="120"/>
+      <c r="S84" s="118"/>
     </row>
     <row r="85" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B85" s="144" t="s">
+      <c r="B85" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="D85" s="122">
+      <c r="D85" s="120">
         <f>STDEV(C80:C83)</f>
         <v>4.0414518746487924E-3</v>
       </c>
-      <c r="F85" s="122">
+      <c r="F85" s="120">
         <f>STDEV(F80:F83)</f>
         <v>3.7318348608439644E-4</v>
       </c>
     </row>
     <row r="86" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="145" t="s">
+      <c r="B86" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="C86" s="147">
+      <c r="C86" s="145">
         <f>MAX(D84:F84)</f>
         <v>8.4596589330132588E-4</v>
       </c>
-      <c r="D86" s="149"/>
-      <c r="E86" s="148"/>
-      <c r="F86" s="124"/>
+      <c r="D86" s="147"/>
+      <c r="E86" s="146"/>
+      <c r="F86" s="122"/>
     </row>
     <row r="90" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B90" s="120" t="s">
+      <c r="B90" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="C90" s="120" t="s">
+      <c r="C90" s="118" t="s">
         <v>83</v>
       </c>
-      <c r="D90" s="120"/>
-      <c r="E90" s="120" t="s">
+      <c r="D90" s="118"/>
+      <c r="E90" s="118" t="s">
         <v>79</v>
       </c>
-      <c r="F90" s="120"/>
+      <c r="F90" s="118"/>
     </row>
     <row r="91" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B91" s="141" t="s">
+      <c r="B91" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="C91" s="142" t="s">
+      <c r="C91" s="140" t="s">
         <v>162</v>
       </c>
-      <c r="D91" s="142" t="s">
+      <c r="D91" s="140" t="s">
         <v>170</v>
       </c>
-      <c r="E91" s="142" t="s">
+      <c r="E91" s="140" t="s">
         <v>169</v>
       </c>
-      <c r="F91" s="143" t="s">
+      <c r="F91" s="141" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="92" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B92" s="144">
+      <c r="B92" s="142">
         <v>1</v>
       </c>
-      <c r="C92" s="140">
+      <c r="C92" s="138">
         <v>370295.05780000001</v>
       </c>
-      <c r="D92" s="150">
+      <c r="D92" s="148">
         <f>$I$12*C92</f>
         <v>30.01698694915223</v>
       </c>
-      <c r="E92" s="122">
+      <c r="E92" s="120">
         <v>16527</v>
       </c>
-      <c r="F92" s="123">
+      <c r="F92" s="121">
         <f>ABS((ABS($I$13)*E92)-$J$13)</f>
         <v>29.990333446391102</v>
       </c>
     </row>
     <row r="93" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B93" s="144">
+      <c r="B93" s="142">
         <v>2</v>
       </c>
-      <c r="C93" s="140">
+      <c r="C93" s="138">
         <v>370295.05080000003</v>
       </c>
-      <c r="D93" s="150">
+      <c r="D93" s="148">
         <f t="shared" ref="D93:D95" si="14">$I$12*C93</f>
         <v>30.016986381715796</v>
       </c>
-      <c r="E93" s="140">
+      <c r="E93" s="138">
         <v>16523</v>
       </c>
-      <c r="F93" s="123">
+      <c r="F93" s="121">
         <f t="shared" ref="F93:F95" si="15">ABS((ABS($I$13)*E93)-$J$13)</f>
         <v>29.9905115444739</v>
       </c>
     </row>
     <row r="94" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B94" s="144">
+      <c r="B94" s="142">
         <v>3</v>
       </c>
-      <c r="C94" s="140">
+      <c r="C94" s="138">
         <v>370295.05780000001</v>
       </c>
-      <c r="D94" s="150">
+      <c r="D94" s="148">
         <f t="shared" si="14"/>
         <v>30.01698694915223</v>
       </c>
-      <c r="E94" s="140">
+      <c r="E94" s="138">
         <v>16516</v>
       </c>
-      <c r="F94" s="123">
+      <c r="F94" s="121">
         <f t="shared" si="15"/>
         <v>29.990823216118802</v>
       </c>
     </row>
     <row r="95" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B95" s="145">
+      <c r="B95" s="143">
         <v>4</v>
       </c>
-      <c r="C95" s="146">
+      <c r="C95" s="144">
         <v>370295.05780000001</v>
       </c>
-      <c r="D95" s="150">
+      <c r="D95" s="148">
         <f t="shared" si="14"/>
         <v>30.01698694915223</v>
       </c>
-      <c r="E95" s="146">
+      <c r="E95" s="144">
         <v>16511</v>
       </c>
-      <c r="F95" s="123">
+      <c r="F95" s="121">
         <f t="shared" si="15"/>
         <v>29.9910458387223</v>
       </c>
     </row>
     <row r="96" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B96" s="141" t="s">
+      <c r="B96" s="139" t="s">
         <v>114</v>
       </c>
-      <c r="D96" s="151">
+      <c r="D96" s="149">
         <f>MAX(D92:D95)-MIN(D92:D95)</f>
         <v>5.6743643384038478E-7</v>
       </c>
-      <c r="F96" s="121">
+      <c r="F96" s="119">
         <f>MAX(F92:F95)-MIN(F92:F95)</f>
         <v>7.1239233119868572E-4</v>
       </c>
     </row>
     <row r="97" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B97" s="144" t="s">
+      <c r="B97" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="D97" s="122">
+      <c r="D97" s="120">
         <f>STDEV(C92:C95)</f>
         <v>3.4999999916180968E-3</v>
       </c>
-      <c r="F97" s="122">
+      <c r="F97" s="120">
         <f>STDEV(F92:F95)</f>
         <v>3.1770879335696334E-4</v>
       </c>
     </row>
     <row r="98" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B98" s="145" t="s">
+      <c r="B98" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="C98" s="147">
+      <c r="C98" s="145">
         <f>MAX(D96:F96)</f>
         <v>7.1239233119868572E-4</v>
       </c>
-      <c r="D98" s="149"/>
-      <c r="E98" s="148"/>
-      <c r="F98" s="124"/>
+      <c r="D98" s="147"/>
+      <c r="E98" s="146"/>
+      <c r="F98" s="122"/>
     </row>
     <row r="102" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B102" s="120" t="s">
+      <c r="B102" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="C102" s="120" t="s">
+      <c r="C102" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="D102" s="120"/>
-      <c r="E102" s="120" t="s">
+      <c r="D102" s="118"/>
+      <c r="E102" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="F102" s="120"/>
+      <c r="F102" s="118"/>
     </row>
     <row r="103" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B103" s="141" t="s">
+      <c r="B103" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="C103" s="142" t="s">
+      <c r="C103" s="140" t="s">
         <v>162</v>
       </c>
-      <c r="D103" s="142" t="s">
+      <c r="D103" s="140" t="s">
         <v>170</v>
       </c>
-      <c r="E103" s="142" t="s">
+      <c r="E103" s="140" t="s">
         <v>169</v>
       </c>
-      <c r="F103" s="143" t="s">
+      <c r="F103" s="141" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="104" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B104" s="144">
+      <c r="B104" s="142">
         <v>1</v>
       </c>
-      <c r="C104" s="140">
+      <c r="C104" s="138">
         <v>493726.6336</v>
       </c>
-      <c r="D104" s="150">
+      <c r="D104" s="148">
         <f>$I$12*C104</f>
         <v>40.022640337869682</v>
       </c>
-      <c r="E104" s="122">
+      <c r="E104" s="120">
         <v>2147276036</v>
       </c>
-      <c r="F104" s="123">
+      <c r="F104" s="121">
         <f>ABS((ABS($I$13)*(2147483647-E104)+$J$13))</f>
         <v>39.969970467047702</v>
       </c>
     </row>
     <row r="105" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B105" s="144">
+      <c r="B105" s="142">
         <v>2</v>
       </c>
-      <c r="C105" s="140">
+      <c r="C105" s="138">
         <v>493726.64059999998</v>
       </c>
-      <c r="D105" s="150">
+      <c r="D105" s="148">
         <f t="shared" ref="D105:D107" si="16">$I$12*C105</f>
         <v>40.022640905306119</v>
       </c>
-      <c r="E105" s="140">
+      <c r="E105" s="138">
         <v>2147276015</v>
       </c>
-      <c r="F105" s="123">
+      <c r="F105" s="121">
         <f t="shared" ref="F105:F107" si="17">ABS((ABS($I$13)*(2147483647-E105)+$J$13))</f>
         <v>39.970905481982399</v>
       </c>
     </row>
     <row r="106" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B106" s="144">
+      <c r="B106" s="142">
         <v>3</v>
       </c>
-      <c r="C106" s="140">
+      <c r="C106" s="138">
         <v>493726.6336</v>
       </c>
-      <c r="D106" s="150">
+      <c r="D106" s="148">
         <f t="shared" si="16"/>
         <v>40.022640337869682</v>
       </c>
-      <c r="E106" s="140">
+      <c r="E106" s="138">
         <v>2147276023</v>
       </c>
-      <c r="F106" s="123">
+      <c r="F106" s="121">
         <f t="shared" si="17"/>
         <v>39.970549285816801</v>
       </c>
-      <c r="K106" s="120"/>
-      <c r="S106" s="120"/>
+      <c r="K106" s="118"/>
+      <c r="S106" s="118"/>
     </row>
     <row r="107" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="145">
+      <c r="B107" s="143">
         <v>4</v>
       </c>
-      <c r="C107" s="146">
+      <c r="C107" s="144">
         <v>493726.64059999998</v>
       </c>
-      <c r="D107" s="150">
+      <c r="D107" s="148">
         <f t="shared" si="16"/>
         <v>40.022640905306119</v>
       </c>
-      <c r="E107" s="146">
+      <c r="E107" s="144">
         <v>2147276027</v>
       </c>
-      <c r="F107" s="123">
+      <c r="F107" s="121">
         <f t="shared" si="17"/>
         <v>39.970371187734003</v>
       </c>
-      <c r="K107" s="120"/>
-      <c r="S107" s="120"/>
+      <c r="K107" s="118"/>
+      <c r="S107" s="118"/>
     </row>
     <row r="108" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B108" s="141" t="s">
+      <c r="B108" s="139" t="s">
         <v>114</v>
       </c>
-      <c r="D108" s="151">
+      <c r="D108" s="149">
         <f>MAX(D104:D107)-MIN(D104:D107)</f>
         <v>5.6743643739309846E-7</v>
       </c>
-      <c r="F108" s="121">
+      <c r="F108" s="119">
         <f>MAX(F104:F107)-MIN(F104:F107)</f>
         <v>9.3501493469716479E-4</v>
       </c>
-      <c r="K108" s="120"/>
-      <c r="S108" s="120"/>
+      <c r="K108" s="118"/>
+      <c r="S108" s="118"/>
     </row>
     <row r="109" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B109" s="144" t="s">
+      <c r="B109" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="D109" s="122">
+      <c r="D109" s="120">
         <f>STDEV(C104:C107)</f>
         <v>4.0414518746487924E-3</v>
       </c>
-      <c r="F109" s="122">
+      <c r="F109" s="120">
         <f>STDEV(F104:F107)</f>
         <v>3.8879366243018771E-4</v>
       </c>
-      <c r="K109" s="120"/>
-      <c r="S109" s="120"/>
+      <c r="K109" s="118"/>
+      <c r="S109" s="118"/>
     </row>
     <row r="110" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B110" s="145" t="s">
+      <c r="B110" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="C110" s="147">
+      <c r="C110" s="145">
         <f>MAX(D108:F108)</f>
         <v>9.3501493469716479E-4</v>
       </c>
-      <c r="D110" s="149"/>
-      <c r="E110" s="148"/>
-      <c r="F110" s="124"/>
-      <c r="K110" s="120"/>
-      <c r="S110" s="120"/>
+      <c r="D110" s="147"/>
+      <c r="E110" s="146"/>
+      <c r="F110" s="122"/>
+      <c r="K110" s="118"/>
+      <c r="S110" s="118"/>
     </row>
     <row r="111" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="K111" s="120"/>
-      <c r="S111" s="120"/>
+      <c r="K111" s="118"/>
+      <c r="S111" s="118"/>
     </row>
     <row r="112" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="K112" s="120"/>
-      <c r="S112" s="120"/>
+      <c r="K112" s="118"/>
+      <c r="S112" s="118"/>
     </row>
     <row r="114" spans="2:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B114" s="120" t="s">
+      <c r="B114" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="C114" s="120" t="s">
+      <c r="C114" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="D114" s="120"/>
-      <c r="E114" s="120" t="s">
+      <c r="D114" s="118"/>
+      <c r="E114" s="118" t="s">
         <v>79</v>
       </c>
-      <c r="F114" s="120"/>
+      <c r="F114" s="118"/>
     </row>
     <row r="115" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B115" s="141" t="s">
+      <c r="B115" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="C115" s="142" t="s">
+      <c r="C115" s="140" t="s">
         <v>162</v>
       </c>
-      <c r="D115" s="142" t="s">
+      <c r="D115" s="140" t="s">
         <v>170</v>
       </c>
-      <c r="E115" s="142" t="s">
+      <c r="E115" s="140" t="s">
         <v>169</v>
       </c>
-      <c r="F115" s="143" t="s">
+      <c r="F115" s="141" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="116" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B116" s="144">
+      <c r="B116" s="142">
         <v>1</v>
       </c>
-      <c r="C116" s="140">
+      <c r="C116" s="138">
         <v>493726.71799999999</v>
       </c>
-      <c r="D116" s="150">
+      <c r="D116" s="148">
         <f>$I$12*C116</f>
         <v>40.02264717953188</v>
       </c>
-      <c r="E116" s="122">
+      <c r="E116" s="120">
         <v>2147275436</v>
       </c>
-      <c r="F116" s="123">
+      <c r="F116" s="121">
         <f>ABS((ABS($I$13)*(2147483647-E116)+$J$13))</f>
         <v>39.996685179467704</v>
       </c>
     </row>
     <row r="117" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B117" s="144">
+      <c r="B117" s="142">
         <v>2</v>
       </c>
-      <c r="C117" s="140">
+      <c r="C117" s="138">
         <v>493726.71799999999</v>
       </c>
-      <c r="D117" s="150">
+      <c r="D117" s="148">
         <f t="shared" ref="D117:D119" si="18">$I$12*C117</f>
         <v>40.02264717953188</v>
       </c>
-      <c r="E117" s="140">
+      <c r="E117" s="138">
         <v>2147275431</v>
       </c>
-      <c r="F117" s="123">
+      <c r="F117" s="121">
         <f t="shared" ref="F117:F119" si="19">ABS((ABS($I$13)*(2147483647-E117)+$J$13))</f>
         <v>39.996907802071199</v>
       </c>
     </row>
     <row r="118" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B118" s="144">
+      <c r="B118" s="142">
         <v>3</v>
       </c>
-      <c r="C118" s="140">
+      <c r="C118" s="138">
         <v>493726.71799999999</v>
       </c>
-      <c r="D118" s="150">
+      <c r="D118" s="148">
         <f t="shared" si="18"/>
         <v>40.02264717953188</v>
       </c>
-      <c r="E118" s="140">
+      <c r="E118" s="138">
         <v>2147275428</v>
       </c>
-      <c r="F118" s="123">
+      <c r="F118" s="121">
         <f t="shared" si="19"/>
         <v>39.997041375633302</v>
       </c>
     </row>
     <row r="119" spans="2:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B119" s="145">
+      <c r="B119" s="143">
         <v>4</v>
       </c>
-      <c r="C119" s="146">
+      <c r="C119" s="144">
         <v>493726.71799999999</v>
       </c>
-      <c r="D119" s="150">
+      <c r="D119" s="148">
         <f t="shared" si="18"/>
         <v>40.02264717953188</v>
       </c>
-      <c r="E119" s="146">
+      <c r="E119" s="144">
         <v>2147275424</v>
       </c>
-      <c r="F119" s="123">
+      <c r="F119" s="121">
         <f t="shared" si="19"/>
         <v>39.9972194737161</v>
       </c>
     </row>
     <row r="120" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B120" s="141" t="s">
+      <c r="B120" s="139" t="s">
         <v>114</v>
       </c>
-      <c r="D120" s="151">
+      <c r="D120" s="149">
         <f>MAX(D116:D119)-MIN(D116:D119)</f>
         <v>0</v>
       </c>
-      <c r="F120" s="121">
+      <c r="F120" s="119">
         <f>MAX(F116:F119)-MIN(F116:F119)</f>
         <v>5.3429424839634976E-4</v>
       </c>
     </row>
     <row r="121" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B121" s="144" t="s">
+      <c r="B121" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="D121" s="122">
+      <c r="D121" s="120">
         <f>STDEV(C116:C119)</f>
         <v>0</v>
       </c>
-      <c r="F121" s="122">
+      <c r="F121" s="120">
         <f>STDEV(F116:F119)</f>
         <v>2.2520489072317337E-4</v>
       </c>
     </row>
     <row r="122" spans="2:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B122" s="145" t="s">
+      <c r="B122" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="C122" s="147">
+      <c r="C122" s="145">
         <f>MAX(D120:F120)</f>
         <v>5.3429424839634976E-4</v>
       </c>
-      <c r="D122" s="149"/>
-      <c r="E122" s="148"/>
-      <c r="F122" s="124"/>
+      <c r="D122" s="147"/>
+      <c r="E122" s="146"/>
+      <c r="F122" s="122"/>
     </row>
     <row r="124" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="M124" s="120"/>
+      <c r="M124" s="118"/>
     </row>
     <row r="125" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="M125" s="120"/>
+      <c r="M125" s="118"/>
     </row>
     <row r="126" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="M126" s="120"/>
+      <c r="M126" s="118"/>
     </row>
     <row r="127" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="M127" s="120"/>
+      <c r="M127" s="118"/>
     </row>
     <row r="128" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="M128" s="120"/>
+      <c r="M128" s="118"/>
     </row>
     <row r="129" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M129" s="120"/>
+      <c r="M129" s="118"/>
     </row>
     <row r="130" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M130" s="120"/>
+      <c r="M130" s="118"/>
     </row>
     <row r="131" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M131" s="120"/>
+      <c r="M131" s="118"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add repeatability data of after collision tests
</commit_message>
<xml_diff>
--- a/docs/testplan/SAT_TEMPLATE_v0_1_after_coll.xlsx
+++ b/docs/testplan/SAT_TEMPLATE_v0_1_after_coll.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="177">
   <si>
     <t>General Inspection</t>
   </si>
@@ -556,6 +556,9 @@
   </si>
   <si>
     <t>Average=</t>
+  </si>
+  <si>
+    <t>Before coll</t>
   </si>
 </sst>
 </file>
@@ -1255,7 +1258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1511,6 +1514,11 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3078,8 +3086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3669,8 +3677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3758,33 +3766,33 @@
         <v>0</v>
       </c>
       <c r="D7" s="84">
-        <f>$I$7*D18</f>
-        <v>-3.4198178189062502E-6</v>
+        <f>($I$7*D18)-$J$7</f>
+        <v>0</v>
       </c>
       <c r="E7" s="84">
-        <f>(ABS($I$8)*E18)-$J$8</f>
-        <v>4.9826375650496857E-2</v>
+        <f>ABS(($I$8)*E18-$J$8)</f>
+        <v>0</v>
       </c>
       <c r="F7" s="84">
         <f>ABS(D7-E7)</f>
-        <v>4.9829795468315764E-2</v>
+        <v>0</v>
       </c>
       <c r="G7" s="107"/>
       <c r="H7" s="77" t="s">
         <v>110</v>
       </c>
       <c r="I7" s="65">
-        <v>8.1062348299999997E-5</v>
-      </c>
-      <c r="J7" s="82">
-        <v>8.1062348299999997E-5</v>
+        <v>8.1016481910443041E-5</v>
+      </c>
+      <c r="J7" s="160">
+        <v>-3.4178828305968161E-6</v>
       </c>
       <c r="K7" s="154" t="s">
         <v>174</v>
       </c>
       <c r="L7" s="155">
         <f>MAX(F7:F11)</f>
-        <v>5.6566004136456627E-2</v>
+        <v>6.4535304828314821E-3</v>
       </c>
       <c r="N7" s="68"/>
       <c r="O7" s="69"/>
@@ -3800,33 +3808,33 @@
         <v>10</v>
       </c>
       <c r="D8" s="84">
-        <f>$I$7*D19</f>
-        <v>10.005657376984987</v>
+        <f t="shared" ref="D8:D11" si="0">($I$7*D19)-$J$7</f>
+        <v>9.9999994318719185</v>
       </c>
       <c r="E8" s="84">
-        <f>ABS((ABS($I$8)*E19)-$J$8)</f>
-        <v>9.9614230547031006</v>
+        <f t="shared" ref="E8:E10" si="1">ABS(($I$8)*E19-$J$8)</f>
+        <v>10.00645296235475</v>
       </c>
       <c r="F8" s="84">
-        <f t="shared" ref="F8:F11" si="0">ABS(D8-E8)</f>
-        <v>4.4234322281885952E-2</v>
+        <f t="shared" ref="F8:F11" si="2">ABS(D8-E8)</f>
+        <v>6.4535304828314821E-3</v>
       </c>
       <c r="G8" s="71"/>
       <c r="H8" s="78" t="s">
         <v>111</v>
       </c>
       <c r="I8" s="40">
-        <v>-4.45245207E-5</v>
+        <v>4.4503188653467018E-5</v>
       </c>
       <c r="J8" s="83">
-        <v>30.726190200000001</v>
+        <v>30.761271545106204</v>
       </c>
       <c r="K8" s="154" t="s">
         <v>175</v>
       </c>
       <c r="L8" s="156">
         <f>AVERAGE(F7:F11)</f>
-        <v>4.9680461078188951E-2</v>
+        <v>3.5337804303164689E-3</v>
       </c>
       <c r="N8" s="58">
         <v>5</v>
@@ -3844,16 +3852,16 @@
         <v>20</v>
       </c>
       <c r="D9" s="84">
-        <f>$I$7*D20</f>
-        <v>20.01131874223751</v>
+        <f t="shared" si="0"/>
+        <v>19.99999943187192</v>
       </c>
       <c r="E9" s="84">
-        <f>ABS((ABS($I$8)*E20)-$J$8)</f>
-        <v>19.966216429555203</v>
+        <f t="shared" si="1"/>
+        <v>20.00645296235475</v>
       </c>
       <c r="F9" s="84">
-        <f t="shared" si="0"/>
-        <v>4.5102312682306689E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.4535304828297058E-3</v>
       </c>
       <c r="G9" s="71"/>
       <c r="N9" s="58"/>
@@ -3870,16 +3878,16 @@
         <v>30</v>
       </c>
       <c r="D10" s="84">
-        <f>$I$7*D21</f>
-        <v>30.016978972617157</v>
+        <f t="shared" si="0"/>
+        <v>29.99999829764117</v>
       </c>
       <c r="E10" s="84">
-        <f>ABS((ABS($I$8)*E21)-$J$8)</f>
-        <v>29.9604129684807</v>
+        <f t="shared" si="1"/>
+        <v>29.995861203455224</v>
       </c>
       <c r="F10" s="84">
-        <f t="shared" si="0"/>
-        <v>5.6566004136456627E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.1370941859462107E-3</v>
       </c>
       <c r="G10" s="71"/>
       <c r="H10" t="s">
@@ -3899,23 +3907,24 @@
         <v>40</v>
       </c>
       <c r="D11" s="84">
-        <f>$I$7*D22</f>
-        <v>40.022640337869682</v>
+        <f t="shared" si="0"/>
+        <v>39.99999829764117</v>
       </c>
       <c r="E11" s="152">
-        <f>ABS((ABS($I$8)*F27)+$J$8)</f>
-        <v>39.969970467047702</v>
+        <f>ABS((ABS($I$8)*(E27-E22)+$J$8))</f>
+        <v>40.000623044641145</v>
       </c>
       <c r="F11" s="84">
-        <f t="shared" si="0"/>
-        <v>5.2669870821979714E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.2474699997494554E-4</v>
       </c>
       <c r="G11" s="71"/>
       <c r="H11" t="s">
         <v>160</v>
       </c>
       <c r="I11">
-        <v>0.99954895683835387</v>
+        <f>ABS(I7-K21)</f>
+        <v>2.4764489556957617E-8</v>
       </c>
       <c r="N11" s="58"/>
       <c r="O11" s="57"/>
@@ -3932,7 +3941,8 @@
         <v>161</v>
       </c>
       <c r="I12">
-        <v>1.0001512578738871</v>
+        <f>ABS(I8-K22)</f>
+        <v>8.2131465329796224E-9</v>
       </c>
       <c r="N12" s="58"/>
       <c r="O12" s="57"/>
@@ -3967,7 +3977,7 @@
       <c r="H16" t="s">
         <v>164</v>
       </c>
-      <c r="I16" s="112">
+      <c r="I16" s="116">
         <v>691207</v>
       </c>
       <c r="J16">
@@ -4030,6 +4040,9 @@
         <v>241664</v>
       </c>
       <c r="F20" s="117"/>
+      <c r="K20" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="21" spans="1:27" s="108" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="51">
@@ -4042,6 +4055,20 @@
         <v>17199</v>
       </c>
       <c r="F21" s="116"/>
+      <c r="H21" s="157">
+        <f>D20-D19</f>
+        <v>123431.67420000001</v>
+      </c>
+      <c r="I21" s="108">
+        <v>10</v>
+      </c>
+      <c r="J21" s="108">
+        <f>10/H21</f>
+        <v>8.1016481910443041E-5</v>
+      </c>
+      <c r="K21" s="108">
+        <v>8.1041246399999998E-5</v>
+      </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C22" s="51">
@@ -4054,6 +4081,17 @@
         <v>2147276036</v>
       </c>
       <c r="F22" s="115"/>
+      <c r="H22" s="158">
+        <f>E19-E20</f>
+        <v>224703</v>
+      </c>
+      <c r="J22">
+        <f>10/H22</f>
+        <v>4.4503188653467018E-5</v>
+      </c>
+      <c r="K22" s="161">
+        <v>4.4511401799999998E-5</v>
+      </c>
     </row>
     <row r="23" spans="1:27" s="79" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23"/>
@@ -4179,14 +4217,14 @@
       <c r="E27">
         <v>2147483647</v>
       </c>
-      <c r="F27" s="153">
-        <f>E27-E22</f>
-        <v>207611</v>
-      </c>
+      <c r="F27" s="153"/>
       <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
-      <c r="J27"/>
+      <c r="J27">
+        <f>E18*$J$22</f>
+        <v>30.761271545106204</v>
+      </c>
       <c r="K27"/>
       <c r="L27"/>
       <c r="M27"/>
@@ -4213,7 +4251,7 @@
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28"/>
-      <c r="H28"/>
+      <c r="H28" s="159"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -4360,7 +4398,6 @@
       <c r="G33"/>
       <c r="H33"/>
       <c r="I33"/>
-      <c r="J33"/>
       <c r="K33"/>
       <c r="L33"/>
       <c r="M33"/>
@@ -4654,8 +4691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4822,9 +4859,7 @@
       <c r="J11" s="88" t="s">
         <v>109</v>
       </c>
-      <c r="K11" s="89" t="s">
-        <v>24</v>
-      </c>
+      <c r="K11" s="89"/>
       <c r="M11"/>
       <c r="N11" s="133"/>
       <c r="O11" s="130"/>
@@ -4842,24 +4877,24 @@
         <v>-4.2187500000000003E-2</v>
       </c>
       <c r="D12" s="148">
-        <f>$I$12*C12</f>
-        <v>-3.4198178189062502E-6</v>
+        <f>($I$12*C12)-$J$12</f>
+        <v>0</v>
       </c>
       <c r="E12" s="120">
         <v>691215</v>
       </c>
       <c r="F12" s="121">
         <f>ABS((ABS($I$13)*E12)-$J$13)</f>
-        <v>4.9826375650496857E-2</v>
+        <v>0</v>
       </c>
       <c r="H12" s="77" t="s">
         <v>110</v>
       </c>
       <c r="I12" s="65">
-        <v>8.1062348299999997E-5</v>
-      </c>
-      <c r="J12" s="82">
-        <v>8.1062348299999997E-5</v>
+        <v>8.1016481910443041E-5</v>
+      </c>
+      <c r="J12" s="160">
+        <v>-3.4178828305968161E-6</v>
       </c>
       <c r="K12" s="80"/>
       <c r="M12"/>
@@ -4879,24 +4914,24 @@
         <v>-4.2187500000000003E-2</v>
       </c>
       <c r="D13" s="148">
-        <f t="shared" ref="D13:D15" si="0">$I$12*C13</f>
-        <v>-3.4198178189062502E-6</v>
+        <f t="shared" ref="D13:D15" si="0">($I$12*C13)-$J$12</f>
+        <v>0</v>
       </c>
       <c r="E13" s="138">
         <v>691212</v>
       </c>
       <c r="F13" s="121">
         <f t="shared" ref="F13:F15" si="1">ABS((ABS($I$13)*E13)-$J$13)</f>
-        <v>4.9692802088397769E-2</v>
+        <v>1.3350956595914454E-4</v>
       </c>
       <c r="H13" s="78" t="s">
         <v>111</v>
       </c>
       <c r="I13" s="40">
-        <v>-4.45245207E-5</v>
+        <v>4.4503188653467018E-5</v>
       </c>
       <c r="J13" s="83">
-        <v>30.726190200000001</v>
+        <v>30.761271545106204</v>
       </c>
       <c r="K13" s="81"/>
       <c r="M13"/>
@@ -4917,14 +4952,14 @@
       </c>
       <c r="D14" s="148">
         <f t="shared" si="0"/>
-        <v>-3.9897874553906247E-6</v>
+        <v>-5.6964713843280219E-7</v>
       </c>
       <c r="E14" s="138">
         <v>691212</v>
       </c>
       <c r="F14" s="121">
         <f t="shared" si="1"/>
-        <v>4.9692802088397769E-2</v>
+        <v>1.3350956595914454E-4</v>
       </c>
       <c r="M14"/>
       <c r="N14" s="133"/>
@@ -4944,14 +4979,14 @@
       </c>
       <c r="D15" s="148">
         <f t="shared" si="0"/>
-        <v>-3.9897874553906247E-6</v>
+        <v>-5.6964713843280219E-7</v>
       </c>
       <c r="E15" s="144">
         <v>691212</v>
       </c>
       <c r="F15" s="121">
         <f t="shared" si="1"/>
-        <v>4.9692802088397769E-2</v>
+        <v>1.3350956595914454E-4</v>
       </c>
       <c r="M15"/>
       <c r="N15" s="133"/>
@@ -4968,11 +5003,11 @@
       </c>
       <c r="D16" s="149">
         <f>MAX(D12:D15)-MIN(D12:D15)</f>
-        <v>5.6996963648437454E-7</v>
+        <v>5.6964713843280219E-7</v>
       </c>
       <c r="F16" s="119">
         <f>MAX(F12:F15)-MIN(F12:F15)</f>
-        <v>1.3357356209908744E-4</v>
+        <v>1.3350956595914454E-4</v>
       </c>
       <c r="M16"/>
       <c r="N16" s="133"/>
@@ -4993,7 +5028,7 @@
       </c>
       <c r="F17" s="120">
         <f>STDEV(F12:F15)</f>
-        <v>6.678678104954372E-5</v>
+        <v>6.6754782979572269E-5</v>
       </c>
       <c r="I17" s="127" t="s">
         <v>117</v>
@@ -5014,7 +5049,7 @@
       </c>
       <c r="C18" s="145">
         <f>MAX(D16:F16)</f>
-        <v>1.3357356209908744E-4</v>
+        <v>1.3350956595914454E-4</v>
       </c>
       <c r="D18" s="147"/>
       <c r="E18" s="146"/>
@@ -5024,7 +5059,7 @@
       </c>
       <c r="I18" s="132">
         <f>MAX(C18,C28,C38,C50,C62,C74,C86,C98,C110,C122)</f>
-        <v>9.3501493469716479E-4</v>
+        <v>9.3456696172466991E-4</v>
       </c>
       <c r="M18"/>
       <c r="N18" s="133"/>
@@ -5042,7 +5077,7 @@
       </c>
       <c r="I19" s="132">
         <f>AVERAGE(C18,C28,C38,C50,C62,C74,C86,C98,C110,C122)</f>
-        <v>6.0108102944944619E-4</v>
+        <v>6.007930468211242E-4</v>
       </c>
       <c r="M19"/>
       <c r="N19" s="133"/>
@@ -5109,15 +5144,15 @@
         <v>4.9218749999999999E-2</v>
       </c>
       <c r="D22" s="148">
-        <f>$I$12*C22</f>
-        <v>3.9897874553906247E-6</v>
+        <f>($I$12*C22)-$J$12</f>
+        <v>7.405412799626434E-6</v>
       </c>
       <c r="E22" s="120">
         <v>690520</v>
       </c>
       <c r="F22" s="121">
         <f>ABS((ABS($I$13)*E22)-$J$13)</f>
-        <v>1.8881833763998657E-2</v>
+        <v>3.0929716114158623E-2</v>
       </c>
       <c r="M22"/>
       <c r="N22" s="133"/>
@@ -5136,15 +5171,15 @@
         <v>4.2187500000000003E-2</v>
       </c>
       <c r="D23" s="148">
-        <f t="shared" ref="D23:D25" si="2">$I$12*C23</f>
-        <v>3.4198178189062502E-6</v>
+        <f t="shared" ref="D23:D25" si="2">($I$12*C23)-$J$12</f>
+        <v>6.8357656611936323E-6</v>
       </c>
       <c r="E23" s="138">
         <v>690512</v>
       </c>
       <c r="F23" s="121">
         <f t="shared" ref="F23:F25" si="3">ABS((ABS($I$13)*E23)-$J$13)</f>
-        <v>1.8525637598397537E-2</v>
+        <v>3.1285741623385377E-2</v>
       </c>
       <c r="M23"/>
       <c r="N23" s="134"/>
@@ -5164,14 +5199,14 @@
       </c>
       <c r="D24" s="148">
         <f t="shared" si="2"/>
-        <v>3.4198178189062502E-6</v>
+        <v>6.8357656611936323E-6</v>
       </c>
       <c r="E24" s="138">
         <v>690511</v>
       </c>
       <c r="F24" s="121">
         <f t="shared" si="3"/>
-        <v>1.8481113077697842E-2</v>
+        <v>3.1330244812039609E-2</v>
       </c>
     </row>
     <row r="25" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -5183,14 +5218,14 @@
       </c>
       <c r="D25" s="148">
         <f t="shared" si="2"/>
-        <v>3.4198178189062502E-6</v>
+        <v>6.8357656611936323E-6</v>
       </c>
       <c r="E25" s="144">
         <v>690507</v>
       </c>
       <c r="F25" s="121">
         <f t="shared" si="3"/>
-        <v>1.8303014994899058E-2</v>
+        <v>3.1508257566652986E-2</v>
       </c>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.3">
@@ -5199,11 +5234,11 @@
       </c>
       <c r="D26" s="149">
         <f>MAX(D22:D25)-MIN(D22:D25)</f>
-        <v>5.6996963648437454E-7</v>
+        <v>5.6964713843280177E-7</v>
       </c>
       <c r="F26" s="119">
         <f>MAX(F22:F25)-MIN(F22:F25)</f>
-        <v>5.7881876909959828E-4</v>
+        <v>5.7854145249436328E-4</v>
       </c>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.3">
@@ -5216,7 +5251,7 @@
       </c>
       <c r="F27" s="120">
         <f>STDEV(F22:F25)</f>
-        <v>2.4251222098224437E-4</v>
+        <v>2.4239603147782865E-4</v>
       </c>
     </row>
     <row r="28" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -5225,7 +5260,7 @@
       </c>
       <c r="C28" s="145">
         <f>MAX(D26:F26)</f>
-        <v>5.7881876909959828E-4</v>
+        <v>5.7854145249436328E-4</v>
       </c>
       <c r="D28" s="147"/>
       <c r="E28" s="146"/>
@@ -5269,15 +5304,15 @@
         <v>123431.625</v>
       </c>
       <c r="D32" s="148">
-        <f>$I$12*C32</f>
-        <v>10.005657376984987</v>
+        <f>($I$12*C32)-$J$12</f>
+        <v>9.9999994318719185</v>
       </c>
       <c r="E32" s="120">
         <v>466367</v>
       </c>
       <c r="F32" s="121">
         <f>ABS((ABS($I$13)*E32)-$J$13)</f>
-        <v>9.9614230547031006</v>
+        <v>10.00645296235475</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.3">
@@ -5288,15 +5323,15 @@
         <v>123431.625</v>
       </c>
       <c r="D33" s="148">
-        <f t="shared" ref="D33:D35" si="4">$I$12*C33</f>
-        <v>10.005657376984987</v>
+        <f t="shared" ref="D33:D35" si="4">($I$12*C33)-$J$12</f>
+        <v>9.9999994318719185</v>
       </c>
       <c r="E33" s="138">
         <v>466352</v>
       </c>
       <c r="F33" s="121">
         <f t="shared" ref="F33:F35" si="5">ABS((ABS($I$13)*E33)-$J$13)</f>
-        <v>9.9620909225136032</v>
+        <v>10.007120510184553</v>
       </c>
       <c r="L33" s="118"/>
     </row>
@@ -5309,14 +5344,14 @@
       </c>
       <c r="D34" s="148">
         <f t="shared" si="4"/>
-        <v>10.005657376984987</v>
+        <v>9.9999994318719185</v>
       </c>
       <c r="E34" s="138">
         <v>466359</v>
       </c>
       <c r="F34" s="121">
         <f t="shared" si="5"/>
-        <v>9.9617792508687018</v>
+        <v>10.00680898786398</v>
       </c>
       <c r="L34" s="124"/>
     </row>
@@ -5329,14 +5364,14 @@
       </c>
       <c r="D35" s="148">
         <f t="shared" si="4"/>
-        <v>10.005657376984987</v>
+        <v>9.9999994318719185</v>
       </c>
       <c r="E35" s="144">
         <v>466363</v>
       </c>
       <c r="F35" s="121">
         <f t="shared" si="5"/>
-        <v>9.961601152785903</v>
+        <v>10.006630975109367</v>
       </c>
       <c r="L35" s="118"/>
     </row>
@@ -5350,7 +5385,7 @@
       </c>
       <c r="F36" s="119">
         <f>MAX(F32:F35)-MIN(F32:F35)</f>
-        <v>6.6786781050254262E-4</v>
+        <v>6.6754782980282812E-4</v>
       </c>
       <c r="L36" s="118"/>
     </row>
@@ -5364,7 +5399,7 @@
       </c>
       <c r="F37" s="120">
         <f>STDEV(F32:F35)</f>
-        <v>2.848061585382772E-4</v>
+        <v>2.8466970567669387E-4</v>
       </c>
       <c r="L37" s="118"/>
     </row>
@@ -5374,7 +5409,7 @@
       </c>
       <c r="C38" s="145">
         <f>MAX(D36:F36)</f>
-        <v>6.6786781050254262E-4</v>
+        <v>6.6754782980282812E-4</v>
       </c>
       <c r="D38" s="147"/>
       <c r="E38" s="146"/>
@@ -5422,15 +5457,15 @@
         <v>123431.70940000001</v>
       </c>
       <c r="D44" s="148">
-        <f>$I$12*C44</f>
-        <v>10.005664218647185</v>
+        <f>($I$12*C44)-$J$12</f>
+        <v>10.000006269662993</v>
       </c>
       <c r="E44" s="120">
         <v>465771</v>
       </c>
       <c r="F44" s="121">
         <f>ABS((ABS($I$13)*E44)-$J$13)</f>
-        <v>9.9879596690403005</v>
+        <v>10.032976862792218</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.3">
@@ -5441,15 +5476,15 @@
         <v>123431.70940000001</v>
       </c>
       <c r="D45" s="148">
-        <f t="shared" ref="D45:D47" si="6">$I$12*C45</f>
-        <v>10.005664218647185</v>
+        <f t="shared" ref="D45:D47" si="6">($I$12*C45)-$J$12</f>
+        <v>10.000006269662993</v>
       </c>
       <c r="E45" s="138">
         <v>465767</v>
       </c>
       <c r="F45" s="121">
         <f t="shared" ref="F45:F47" si="7">ABS((ABS($I$13)*E45)-$J$13)</f>
-        <v>9.9881377671231029</v>
+        <v>10.033154875546831</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.3">
@@ -5461,14 +5496,14 @@
       </c>
       <c r="D46" s="148">
         <f t="shared" si="6"/>
-        <v>10.005664218647185</v>
+        <v>10.000006269662993</v>
       </c>
       <c r="E46" s="138">
         <v>465763</v>
       </c>
       <c r="F46" s="121">
         <f t="shared" si="7"/>
-        <v>9.9883158652059016</v>
+        <v>10.033332888301445</v>
       </c>
     </row>
     <row r="47" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -5480,14 +5515,14 @@
       </c>
       <c r="D47" s="148">
         <f t="shared" si="6"/>
-        <v>10.005664786083623</v>
+        <v>10.000006836778367</v>
       </c>
       <c r="E47" s="144">
         <v>465759</v>
       </c>
       <c r="F47" s="121">
         <f t="shared" si="7"/>
-        <v>9.9884939632887004</v>
+        <v>10.033510901056058</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.3">
@@ -5496,11 +5531,11 @@
       </c>
       <c r="D48" s="149">
         <f>MAX(D44:D47)-MIN(D44:D47)</f>
-        <v>5.6743643739309846E-7</v>
+        <v>5.6711537332887474E-7</v>
       </c>
       <c r="F48" s="119">
         <f>MAX(F44:F47)-MIN(F44:F47)</f>
-        <v>5.3429424839990247E-4</v>
+        <v>5.3403826384013087E-4</v>
       </c>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.3">
@@ -5513,7 +5548,7 @@
       </c>
       <c r="F49" s="120">
         <f>STDEV(F44:F47)</f>
-        <v>2.29923636225095E-4</v>
+        <v>2.2981347801003879E-4</v>
       </c>
     </row>
     <row r="50" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -5522,7 +5557,7 @@
       </c>
       <c r="C50" s="145">
         <f>MAX(D48:F48)</f>
-        <v>5.3429424839990247E-4</v>
+        <v>5.3403826384013087E-4</v>
       </c>
       <c r="D50" s="147"/>
       <c r="E50" s="146"/>
@@ -5566,15 +5601,15 @@
         <v>246863.29920000001</v>
       </c>
       <c r="D56" s="148">
-        <f>$I$12*C56</f>
-        <v>20.01131874223751</v>
+        <f>($I$12*C56)-$J$12</f>
+        <v>19.99999943187192</v>
       </c>
       <c r="E56" s="120">
         <v>241664</v>
       </c>
       <c r="F56" s="121">
         <f>ABS((ABS($I$13)*E56)-$J$13)</f>
-        <v>19.966216429555203</v>
+        <v>20.00645296235475</v>
       </c>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.3">
@@ -5585,15 +5620,15 @@
         <v>246863.2922</v>
       </c>
       <c r="D57" s="148">
-        <f t="shared" ref="D57:D59" si="8">$I$12*C57</f>
-        <v>20.011318174801072</v>
+        <f t="shared" ref="D57:D59" si="8">($I$12*C57)-$J$12</f>
+        <v>19.999998864756545</v>
       </c>
       <c r="E57" s="138">
         <v>241656</v>
       </c>
       <c r="F57" s="121">
         <f t="shared" ref="F57:F59" si="9">ABS((ABS($I$13)*E57)-$J$13)</f>
-        <v>19.966572625720801</v>
+        <v>20.006808987863977</v>
       </c>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.3">
@@ -5605,14 +5640,14 @@
       </c>
       <c r="D58" s="148">
         <f t="shared" si="8"/>
-        <v>20.01131874223751</v>
+        <v>19.99999943187192</v>
       </c>
       <c r="E58" s="138">
         <v>241663</v>
       </c>
       <c r="F58" s="121">
         <f t="shared" si="9"/>
-        <v>19.966260954075899</v>
+        <v>20.006497465543404</v>
       </c>
       <c r="K58" s="118"/>
       <c r="S58" s="118"/>
@@ -5626,14 +5661,14 @@
       </c>
       <c r="D59" s="148">
         <f t="shared" si="8"/>
-        <v>20.01131874223751</v>
+        <v>19.99999943187192</v>
       </c>
       <c r="E59" s="144">
         <v>241668</v>
       </c>
       <c r="F59" s="121">
         <f t="shared" si="9"/>
-        <v>19.966038331472401</v>
+        <v>20.006274949600137</v>
       </c>
       <c r="K59" s="124"/>
       <c r="S59" s="118"/>
@@ -5644,11 +5679,11 @@
       </c>
       <c r="D60" s="149">
         <f>MAX(D56:D59)-MIN(D56:D59)</f>
-        <v>5.6743643739309846E-7</v>
+        <v>5.6711537510523158E-7</v>
       </c>
       <c r="F60" s="119">
         <f>MAX(F56:F59)-MIN(F56:F59)</f>
-        <v>5.3429424839990247E-4</v>
+        <v>5.3403826384013087E-4</v>
       </c>
       <c r="K60" s="118"/>
       <c r="S60" s="118"/>
@@ -5663,7 +5698,7 @@
       </c>
       <c r="F61" s="120">
         <f>STDEV(F56:F59)</f>
-        <v>2.2225125611281983E-4</v>
+        <v>2.2214477379518184E-4</v>
       </c>
       <c r="K61" s="118"/>
       <c r="S61" s="118"/>
@@ -5674,7 +5709,7 @@
       </c>
       <c r="C62" s="145">
         <f>MAX(D60:F60)</f>
-        <v>5.3429424839990247E-4</v>
+        <v>5.3403826384013087E-4</v>
       </c>
       <c r="D62" s="147"/>
       <c r="E62" s="146"/>
@@ -5728,15 +5763,15 @@
         <v>246863.3836</v>
       </c>
       <c r="D68" s="148">
-        <f>$I$12*C68</f>
-        <v>20.011325583899708</v>
+        <f>($I$12*C68)-$J$12</f>
+        <v>20.00000626966299</v>
       </c>
       <c r="E68" s="120">
         <v>241192</v>
       </c>
       <c r="F68" s="121">
         <f>ABS((ABS($I$13)*E68)-$J$13)</f>
-        <v>19.987232003325602</v>
+        <v>20.027458467399185</v>
       </c>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.3">
@@ -5747,15 +5782,15 @@
         <v>246863.3836</v>
       </c>
       <c r="D69" s="148">
-        <f t="shared" ref="D69:D71" si="10">$I$12*C69</f>
-        <v>20.011325583899708</v>
+        <f t="shared" ref="D69:D71" si="10">($I$12*C69)-$J$12</f>
+        <v>20.00000626966299</v>
       </c>
       <c r="E69" s="138">
         <v>241188</v>
       </c>
       <c r="F69" s="121">
         <f t="shared" ref="F69:F71" si="11">ABS((ABS($I$13)*E69)-$J$13)</f>
-        <v>19.9874101014084</v>
+        <v>20.027636480153802</v>
       </c>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.3">
@@ -5767,14 +5802,14 @@
       </c>
       <c r="D70" s="148">
         <f t="shared" si="10"/>
-        <v>20.011325583899708</v>
+        <v>20.00000626966299</v>
       </c>
       <c r="E70" s="138">
         <v>241184</v>
       </c>
       <c r="F70" s="121">
         <f t="shared" si="11"/>
-        <v>19.987588199491199</v>
+        <v>20.027814492908416</v>
       </c>
     </row>
     <row r="71" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -5786,14 +5821,14 @@
       </c>
       <c r="D71" s="148">
         <f t="shared" si="10"/>
-        <v>20.011325583899708</v>
+        <v>20.00000626966299</v>
       </c>
       <c r="E71" s="144">
         <v>241180</v>
       </c>
       <c r="F71" s="121">
         <f t="shared" si="11"/>
-        <v>19.987766297574002</v>
+        <v>20.027992505663029</v>
       </c>
     </row>
     <row r="72" spans="2:19" x14ac:dyDescent="0.3">
@@ -5806,7 +5841,7 @@
       </c>
       <c r="F72" s="119">
         <f>MAX(F68:F71)-MIN(F68:F71)</f>
-        <v>5.3429424839990247E-4</v>
+        <v>5.3403826384368358E-4</v>
       </c>
     </row>
     <row r="73" spans="2:19" x14ac:dyDescent="0.3">
@@ -5819,7 +5854,7 @@
       </c>
       <c r="F73" s="120">
         <f>STDEV(F68:F71)</f>
-        <v>2.29923636225095E-4</v>
+        <v>2.2981347801141478E-4</v>
       </c>
     </row>
     <row r="74" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -5828,7 +5863,7 @@
       </c>
       <c r="C74" s="145">
         <f>MAX(D72:F72)</f>
-        <v>5.3429424839990247E-4</v>
+        <v>5.3403826384368358E-4</v>
       </c>
       <c r="D74" s="147"/>
       <c r="E74" s="146"/>
@@ -5877,15 +5912,15 @@
         <v>370294.95939999999</v>
       </c>
       <c r="D80" s="148">
-        <f>$I$12*C80</f>
-        <v>30.016978972617157</v>
+        <f>($I$12*C80)-$J$12</f>
+        <v>29.99999829764117</v>
       </c>
       <c r="E80" s="120">
         <v>17199</v>
       </c>
       <c r="F80" s="121">
         <f>ABS((ABS($I$13)*E80)-$J$13)</f>
-        <v>29.9604129684807</v>
+        <v>29.995861203455224</v>
       </c>
       <c r="S80" s="118"/>
     </row>
@@ -5897,15 +5932,15 @@
         <v>370294.95939999999</v>
       </c>
       <c r="D81" s="148">
-        <f t="shared" ref="D81:D83" si="12">$I$12*C81</f>
-        <v>30.016978972617157</v>
+        <f t="shared" ref="D81:D83" si="12">($I$12*C81)-$J$12</f>
+        <v>29.99999829764117</v>
       </c>
       <c r="E81" s="138">
         <v>17180</v>
       </c>
       <c r="F81" s="121">
         <f t="shared" ref="F81:F83" si="13">ABS((ABS($I$13)*E81)-$J$13)</f>
-        <v>29.961258934374001</v>
+        <v>29.99670676403964</v>
       </c>
       <c r="S81" s="118"/>
     </row>
@@ -5918,14 +5953,14 @@
       </c>
       <c r="D82" s="148">
         <f t="shared" si="12"/>
-        <v>30.016979540053594</v>
+        <v>29.999998864756542</v>
       </c>
       <c r="E82" s="138">
         <v>17184</v>
       </c>
       <c r="F82" s="121">
         <f t="shared" si="13"/>
-        <v>29.961080836291202</v>
+        <v>29.996528751285027</v>
       </c>
       <c r="S82" s="118"/>
     </row>
@@ -5938,14 +5973,14 @@
       </c>
       <c r="D83" s="148">
         <f t="shared" si="12"/>
-        <v>30.016979540053594</v>
+        <v>29.999998864756542</v>
       </c>
       <c r="E83" s="144">
         <v>17184</v>
       </c>
       <c r="F83" s="121">
         <f t="shared" si="13"/>
-        <v>29.961080836291202</v>
+        <v>29.996528751285027</v>
       </c>
       <c r="S83" s="118"/>
     </row>
@@ -5955,11 +5990,11 @@
       </c>
       <c r="D84" s="149">
         <f>MAX(D80:D83)-MIN(D80:D83)</f>
-        <v>5.6743643739309846E-7</v>
+        <v>5.671153715525179E-7</v>
       </c>
       <c r="F84" s="119">
         <f>MAX(F80:F83)-MIN(F80:F83)</f>
-        <v>8.4596589330132588E-4</v>
+        <v>8.4556058441620507E-4</v>
       </c>
       <c r="S84" s="118"/>
     </row>
@@ -5973,7 +6008,7 @@
       </c>
       <c r="F85" s="120">
         <f>STDEV(F80:F83)</f>
-        <v>3.7318348608439644E-4</v>
+        <v>3.7300469095322044E-4</v>
       </c>
     </row>
     <row r="86" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -5982,7 +6017,7 @@
       </c>
       <c r="C86" s="145">
         <f>MAX(D84:F84)</f>
-        <v>8.4596589330132588E-4</v>
+        <v>8.4556058441620507E-4</v>
       </c>
       <c r="D86" s="147"/>
       <c r="E86" s="146"/>
@@ -6026,15 +6061,15 @@
         <v>370295.05780000001</v>
       </c>
       <c r="D92" s="148">
-        <f>$I$12*C92</f>
-        <v>30.01698694915223</v>
+        <f>($I$12*C92)-$J$12</f>
+        <v>30.00000626966299</v>
       </c>
       <c r="E92" s="120">
         <v>16527</v>
       </c>
       <c r="F92" s="121">
         <f>ABS((ABS($I$13)*E92)-$J$13)</f>
-        <v>29.990333446391102</v>
+        <v>30.025767346230356</v>
       </c>
     </row>
     <row r="93" spans="2:19" x14ac:dyDescent="0.3">
@@ -6045,15 +6080,15 @@
         <v>370295.05080000003</v>
       </c>
       <c r="D93" s="148">
-        <f t="shared" ref="D93:D95" si="14">$I$12*C93</f>
-        <v>30.016986381715796</v>
+        <f t="shared" ref="D93:D95" si="14">($I$12*C93)-$J$12</f>
+        <v>30.000005702547618</v>
       </c>
       <c r="E93" s="138">
         <v>16523</v>
       </c>
       <c r="F93" s="121">
         <f t="shared" ref="F93:F95" si="15">ABS((ABS($I$13)*E93)-$J$13)</f>
-        <v>29.9905115444739</v>
+        <v>30.02594535898497</v>
       </c>
     </row>
     <row r="94" spans="2:19" x14ac:dyDescent="0.3">
@@ -6065,14 +6100,14 @@
       </c>
       <c r="D94" s="148">
         <f t="shared" si="14"/>
-        <v>30.01698694915223</v>
+        <v>30.00000626966299</v>
       </c>
       <c r="E94" s="138">
         <v>16516</v>
       </c>
       <c r="F94" s="121">
         <f t="shared" si="15"/>
-        <v>29.990823216118802</v>
+        <v>30.026256881305542</v>
       </c>
     </row>
     <row r="95" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -6084,14 +6119,14 @@
       </c>
       <c r="D95" s="148">
         <f t="shared" si="14"/>
-        <v>30.01698694915223</v>
+        <v>30.00000626966299</v>
       </c>
       <c r="E95" s="144">
         <v>16511</v>
       </c>
       <c r="F95" s="121">
         <f t="shared" si="15"/>
-        <v>29.9910458387223</v>
+        <v>30.02647939724881</v>
       </c>
     </row>
     <row r="96" spans="2:19" x14ac:dyDescent="0.3">
@@ -6100,11 +6135,11 @@
       </c>
       <c r="D96" s="149">
         <f>MAX(D92:D95)-MIN(D92:D95)</f>
-        <v>5.6743643384038478E-7</v>
+        <v>5.671153715525179E-7</v>
       </c>
       <c r="F96" s="119">
         <f>MAX(F92:F95)-MIN(F92:F95)</f>
-        <v>7.1239233119868572E-4</v>
+        <v>7.1205101845350782E-4</v>
       </c>
     </row>
     <row r="97" spans="2:19" x14ac:dyDescent="0.3">
@@ -6117,7 +6152,7 @@
       </c>
       <c r="F97" s="120">
         <f>STDEV(F92:F95)</f>
-        <v>3.1770879335696334E-4</v>
+        <v>3.1755657658538152E-4</v>
       </c>
     </row>
     <row r="98" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -6126,7 +6161,7 @@
       </c>
       <c r="C98" s="145">
         <f>MAX(D96:F96)</f>
-        <v>7.1239233119868572E-4</v>
+        <v>7.1205101845350782E-4</v>
       </c>
       <c r="D98" s="147"/>
       <c r="E98" s="146"/>
@@ -6170,15 +6205,15 @@
         <v>493726.6336</v>
       </c>
       <c r="D104" s="148">
-        <f>$I$12*C104</f>
-        <v>40.022640337869682</v>
+        <f>($I$12*C104)-$J$12</f>
+        <v>39.99999829764117</v>
       </c>
       <c r="E104" s="120">
         <v>2147276036</v>
       </c>
       <c r="F104" s="121">
         <f>ABS((ABS($I$13)*(2147483647-E104)+$J$13))</f>
-        <v>39.969970467047702</v>
+        <v>40.000623044641145</v>
       </c>
     </row>
     <row r="105" spans="2:19" x14ac:dyDescent="0.3">
@@ -6189,15 +6224,15 @@
         <v>493726.64059999998</v>
       </c>
       <c r="D105" s="148">
-        <f t="shared" ref="D105:D107" si="16">$I$12*C105</f>
-        <v>40.022640905306119</v>
+        <f t="shared" ref="D105:D107" si="16">($I$12*C105)-$J$12</f>
+        <v>39.999998864756542</v>
       </c>
       <c r="E105" s="138">
         <v>2147276015</v>
       </c>
       <c r="F105" s="121">
         <f t="shared" ref="F105:F107" si="17">ABS((ABS($I$13)*(2147483647-E105)+$J$13))</f>
-        <v>39.970905481982399</v>
+        <v>40.00155761160287</v>
       </c>
     </row>
     <row r="106" spans="2:19" x14ac:dyDescent="0.3">
@@ -6209,14 +6244,14 @@
       </c>
       <c r="D106" s="148">
         <f t="shared" si="16"/>
-        <v>40.022640337869682</v>
+        <v>39.99999829764117</v>
       </c>
       <c r="E106" s="138">
         <v>2147276023</v>
       </c>
       <c r="F106" s="121">
         <f t="shared" si="17"/>
-        <v>39.970549285816801</v>
+        <v>40.001201586093643</v>
       </c>
       <c r="K106" s="118"/>
       <c r="S106" s="118"/>
@@ -6230,14 +6265,14 @@
       </c>
       <c r="D107" s="148">
         <f t="shared" si="16"/>
-        <v>40.022640905306119</v>
+        <v>39.999998864756542</v>
       </c>
       <c r="E107" s="144">
         <v>2147276027</v>
       </c>
       <c r="F107" s="121">
         <f t="shared" si="17"/>
-        <v>39.970371187734003</v>
+        <v>40.001023573339026</v>
       </c>
       <c r="K107" s="118"/>
       <c r="S107" s="118"/>
@@ -6248,11 +6283,11 @@
       </c>
       <c r="D108" s="149">
         <f>MAX(D104:D107)-MIN(D104:D107)</f>
-        <v>5.6743643739309846E-7</v>
+        <v>5.671153715525179E-7</v>
       </c>
       <c r="F108" s="119">
         <f>MAX(F104:F107)-MIN(F104:F107)</f>
-        <v>9.3501493469716479E-4</v>
+        <v>9.3456696172466991E-4</v>
       </c>
       <c r="K108" s="118"/>
       <c r="S108" s="118"/>
@@ -6267,7 +6302,7 @@
       </c>
       <c r="F109" s="120">
         <f>STDEV(F104:F107)</f>
-        <v>3.8879366243018771E-4</v>
+        <v>3.8860738834411117E-4</v>
       </c>
       <c r="K109" s="118"/>
       <c r="S109" s="118"/>
@@ -6278,7 +6313,7 @@
       </c>
       <c r="C110" s="145">
         <f>MAX(D108:F108)</f>
-        <v>9.3501493469716479E-4</v>
+        <v>9.3456696172466991E-4</v>
       </c>
       <c r="D110" s="147"/>
       <c r="E110" s="146"/>
@@ -6332,15 +6367,15 @@
         <v>493726.71799999999</v>
       </c>
       <c r="D116" s="148">
-        <f>$I$12*C116</f>
-        <v>40.02264717953188</v>
+        <f>($I$12*C116)-$J$12</f>
+        <v>40.000005135432239</v>
       </c>
       <c r="E116" s="120">
         <v>2147275436</v>
       </c>
       <c r="F116" s="121">
         <f>ABS((ABS($I$13)*(2147483647-E116)+$J$13))</f>
-        <v>39.996685179467704</v>
+        <v>40.02732495783323</v>
       </c>
     </row>
     <row r="117" spans="2:13" x14ac:dyDescent="0.3">
@@ -6351,15 +6386,15 @@
         <v>493726.71799999999</v>
       </c>
       <c r="D117" s="148">
-        <f t="shared" ref="D117:D119" si="18">$I$12*C117</f>
-        <v>40.02264717953188</v>
+        <f t="shared" ref="D117:D119" si="18">($I$12*C117)-$J$12</f>
+        <v>40.000005135432239</v>
       </c>
       <c r="E117" s="138">
         <v>2147275431</v>
       </c>
       <c r="F117" s="121">
         <f t="shared" ref="F117:F119" si="19">ABS((ABS($I$13)*(2147483647-E117)+$J$13))</f>
-        <v>39.996907802071199</v>
+        <v>40.027547473776494</v>
       </c>
     </row>
     <row r="118" spans="2:13" x14ac:dyDescent="0.3">
@@ -6371,14 +6406,14 @@
       </c>
       <c r="D118" s="148">
         <f t="shared" si="18"/>
-        <v>40.02264717953188</v>
+        <v>40.000005135432239</v>
       </c>
       <c r="E118" s="138">
         <v>2147275428</v>
       </c>
       <c r="F118" s="121">
         <f t="shared" si="19"/>
-        <v>39.997041375633302</v>
+        <v>40.027680983342449</v>
       </c>
     </row>
     <row r="119" spans="2:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -6390,14 +6425,14 @@
       </c>
       <c r="D119" s="148">
         <f t="shared" si="18"/>
-        <v>40.02264717953188</v>
+        <v>40.000005135432239</v>
       </c>
       <c r="E119" s="144">
         <v>2147275424</v>
       </c>
       <c r="F119" s="121">
         <f t="shared" si="19"/>
-        <v>39.9972194737161</v>
+        <v>40.027858996097066</v>
       </c>
     </row>
     <row r="120" spans="2:13" x14ac:dyDescent="0.3">
@@ -6410,7 +6445,7 @@
       </c>
       <c r="F120" s="119">
         <f>MAX(F116:F119)-MIN(F116:F119)</f>
-        <v>5.3429424839634976E-4</v>
+        <v>5.3403826383657815E-4</v>
       </c>
     </row>
     <row r="121" spans="2:13" x14ac:dyDescent="0.3">
@@ -6423,7 +6458,7 @@
       </c>
       <c r="F121" s="120">
         <f>STDEV(F116:F119)</f>
-        <v>2.2520489072317337E-4</v>
+        <v>2.250969932951564E-4</v>
       </c>
     </row>
     <row r="122" spans="2:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -6432,7 +6467,7 @@
       </c>
       <c r="C122" s="145">
         <f>MAX(D120:F120)</f>
-        <v>5.3429424839634976E-4</v>
+        <v>5.3403826383657815E-4</v>
       </c>
       <c r="D122" s="147"/>
       <c r="E122" s="146"/>

</xml_diff>